<commit_message>
[MS-WEBSS] Add new cases and capture code for 9 fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source Depot\Repos\Interop-TestSuites-1\SharePoint\Docs\MS-WEBSS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="360" windowWidth="15405" windowHeight="6600" tabRatio="570"/>
   </bookViews>
@@ -7675,7 +7680,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7958,20 +7963,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7997,444 +7990,189 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="41">
     <dxf>
       <font>
-        <strike/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
-      <font>
-        <strike/>
-      </font>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -8611,168 +8349,121 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <strike/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <strike/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <strike/>
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <strike/>
+      </font>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
       </font>
     </dxf>
   </dxfs>
@@ -8904,34 +8595,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I954" tableType="xml" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I954" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I954"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="92">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="91">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="90">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="89">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="88">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="87">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="86">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="85">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="84">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8940,12 +8631,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101" tableBorderDxfId="99" totalsRowBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="97"/>
-    <tableColumn id="2" name="Test" dataDxfId="96"/>
-    <tableColumn id="3" name="Description" dataDxfId="95"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8994,7 +8685,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9027,9 +8718,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9062,6 +8770,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9245,15 +8970,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="22.25" style="9" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
     <col min="3" max="3" width="85" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
     <col min="8" max="8" width="23" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="2" customWidth="1"/>
     <col min="10" max="11" width="9" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
@@ -9295,127 +9020,127 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -9428,12 +9153,12 @@
       <c r="C12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10">
@@ -9446,12 +9171,12 @@
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">
@@ -9464,12 +9189,12 @@
       <c r="C14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10">
@@ -9482,60 +9207,60 @@
       <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="30">
+    <row r="16" spans="1:10">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="43" t="s">
         <v>1957</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="30">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="4"/>
       <c r="L18" s="3"/>
     </row>
@@ -9621,7 +9346,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="21" customFormat="1" ht="30">
+    <row r="22" spans="1:12" s="21" customFormat="1">
       <c r="A22" s="20" t="s">
         <v>46</v>
       </c>
@@ -9721,7 +9446,7 @@
       </c>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:12" s="21" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="21" customFormat="1">
       <c r="A26" s="20" t="s">
         <v>50</v>
       </c>
@@ -9846,7 +9571,7 @@
       </c>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:12" s="21" customFormat="1" ht="30">
+    <row r="31" spans="1:12" s="21" customFormat="1">
       <c r="A31" s="20" t="s">
         <v>55</v>
       </c>
@@ -10021,7 +9746,7 @@
       </c>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" spans="1:9" ht="30">
+    <row r="38" spans="1:9">
       <c r="A38" s="28" t="s">
         <v>62</v>
       </c>
@@ -10071,7 +9796,7 @@
       </c>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9">
       <c r="A40" s="28" t="s">
         <v>64</v>
       </c>
@@ -10171,7 +9896,7 @@
       </c>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9">
       <c r="A44" s="28" t="s">
         <v>68</v>
       </c>
@@ -10221,7 +9946,7 @@
       </c>
       <c r="I45" s="30"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9">
       <c r="A46" s="28" t="s">
         <v>70</v>
       </c>
@@ -10246,7 +9971,7 @@
       </c>
       <c r="I46" s="30"/>
     </row>
-    <row r="47" spans="1:9" ht="45">
+    <row r="47" spans="1:9" ht="30">
       <c r="A47" s="28" t="s">
         <v>71</v>
       </c>
@@ -10298,7 +10023,7 @@
       </c>
       <c r="I48" s="30"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9">
       <c r="A49" s="28" t="s">
         <v>73</v>
       </c>
@@ -10423,7 +10148,7 @@
       </c>
       <c r="I53" s="30"/>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9">
       <c r="A54" s="28" t="s">
         <v>78</v>
       </c>
@@ -10473,7 +10198,7 @@
       </c>
       <c r="I55" s="18"/>
     </row>
-    <row r="56" spans="1:9" ht="45">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="28" t="s">
         <v>80</v>
       </c>
@@ -10500,7 +10225,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="30">
       <c r="A57" s="28" t="s">
         <v>81</v>
       </c>
@@ -10527,7 +10252,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="45">
+    <row r="58" spans="1:9" ht="30">
       <c r="A58" s="28" t="s">
         <v>82</v>
       </c>
@@ -10554,7 +10279,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="45">
+    <row r="59" spans="1:9" ht="30">
       <c r="A59" s="28" t="s">
         <v>83</v>
       </c>
@@ -10581,7 +10306,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="28" t="s">
         <v>84</v>
       </c>
@@ -10658,7 +10383,7 @@
       </c>
       <c r="I62" s="30"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9">
       <c r="A63" s="28" t="s">
         <v>87</v>
       </c>
@@ -10683,7 +10408,7 @@
       </c>
       <c r="I63" s="30"/>
     </row>
-    <row r="64" spans="1:9" ht="30">
+    <row r="64" spans="1:9">
       <c r="A64" s="28" t="s">
         <v>88</v>
       </c>
@@ -10708,7 +10433,7 @@
       </c>
       <c r="I64" s="30"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9">
       <c r="A65" s="28" t="s">
         <v>89</v>
       </c>
@@ -10733,7 +10458,7 @@
       </c>
       <c r="I65" s="30"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9">
       <c r="A66" s="28" t="s">
         <v>90</v>
       </c>
@@ -10833,7 +10558,7 @@
       </c>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9">
       <c r="A70" s="28" t="s">
         <v>94</v>
       </c>
@@ -10858,7 +10583,7 @@
       </c>
       <c r="I70" s="18"/>
     </row>
-    <row r="71" spans="1:9" ht="90">
+    <row r="71" spans="1:9" ht="75">
       <c r="A71" s="28" t="s">
         <v>95</v>
       </c>
@@ -10883,7 +10608,7 @@
       </c>
       <c r="I71" s="18"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9">
       <c r="A72" s="28" t="s">
         <v>96</v>
       </c>
@@ -11108,7 +10833,7 @@
       </c>
       <c r="I80" s="30"/>
     </row>
-    <row r="81" spans="1:9" ht="45">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="20" t="s">
         <v>105</v>
       </c>
@@ -11133,7 +10858,7 @@
       </c>
       <c r="I81" s="30"/>
     </row>
-    <row r="82" spans="1:9" ht="60">
+    <row r="82" spans="1:9" ht="45">
       <c r="A82" s="20" t="s">
         <v>106</v>
       </c>
@@ -11258,7 +10983,7 @@
       </c>
       <c r="I86" s="30"/>
     </row>
-    <row r="87" spans="1:9" ht="45">
+    <row r="87" spans="1:9" ht="30">
       <c r="A87" s="28" t="s">
         <v>111</v>
       </c>
@@ -11283,7 +11008,7 @@
       </c>
       <c r="I87" s="30"/>
     </row>
-    <row r="88" spans="1:9" ht="45">
+    <row r="88" spans="1:9" ht="30">
       <c r="A88" s="28" t="s">
         <v>112</v>
       </c>
@@ -11308,7 +11033,7 @@
       </c>
       <c r="I88" s="30"/>
     </row>
-    <row r="89" spans="1:9" ht="45">
+    <row r="89" spans="1:9" ht="30">
       <c r="A89" s="28" t="s">
         <v>113</v>
       </c>
@@ -11608,7 +11333,7 @@
       </c>
       <c r="I100" s="30"/>
     </row>
-    <row r="101" spans="1:9" ht="45">
+    <row r="101" spans="1:9" ht="30">
       <c r="A101" s="28" t="s">
         <v>125</v>
       </c>
@@ -12233,7 +11958,7 @@
       </c>
       <c r="I125" s="30"/>
     </row>
-    <row r="126" spans="1:9" ht="45">
+    <row r="126" spans="1:9" ht="30">
       <c r="A126" s="28" t="s">
         <v>150</v>
       </c>
@@ -12258,7 +11983,7 @@
       </c>
       <c r="I126" s="30"/>
     </row>
-    <row r="127" spans="1:9" ht="45">
+    <row r="127" spans="1:9" ht="30">
       <c r="A127" s="28" t="s">
         <v>151</v>
       </c>
@@ -12333,7 +12058,7 @@
       </c>
       <c r="I129" s="30"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9">
       <c r="A130" s="28" t="s">
         <v>154</v>
       </c>
@@ -12383,7 +12108,7 @@
       </c>
       <c r="I131" s="30"/>
     </row>
-    <row r="132" spans="1:9" ht="45">
+    <row r="132" spans="1:9" ht="30">
       <c r="A132" s="28" t="s">
         <v>156</v>
       </c>
@@ -12435,7 +12160,7 @@
       </c>
       <c r="I133" s="30"/>
     </row>
-    <row r="134" spans="1:9" ht="45">
+    <row r="134" spans="1:9" ht="30">
       <c r="A134" s="28" t="s">
         <v>158</v>
       </c>
@@ -12535,7 +12260,7 @@
       </c>
       <c r="I137" s="30"/>
     </row>
-    <row r="138" spans="1:9" ht="45">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="28" t="s">
         <v>162</v>
       </c>
@@ -12560,7 +12285,7 @@
       </c>
       <c r="I138" s="18"/>
     </row>
-    <row r="139" spans="1:9" ht="45">
+    <row r="139" spans="1:9" ht="30">
       <c r="A139" s="28" t="s">
         <v>163</v>
       </c>
@@ -12610,7 +12335,7 @@
       </c>
       <c r="I140" s="30"/>
     </row>
-    <row r="141" spans="1:9" ht="45">
+    <row r="141" spans="1:9" ht="30">
       <c r="A141" s="28" t="s">
         <v>165</v>
       </c>
@@ -12635,7 +12360,7 @@
       </c>
       <c r="I141" s="18"/>
     </row>
-    <row r="142" spans="1:9" ht="45">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="28" t="s">
         <v>166</v>
       </c>
@@ -12860,7 +12585,7 @@
       </c>
       <c r="I150" s="30"/>
     </row>
-    <row r="151" spans="1:9" ht="30">
+    <row r="151" spans="1:9">
       <c r="A151" s="28" t="s">
         <v>175</v>
       </c>
@@ -12935,7 +12660,7 @@
       </c>
       <c r="I153" s="30"/>
     </row>
-    <row r="154" spans="1:9" ht="45">
+    <row r="154" spans="1:9" ht="30">
       <c r="A154" s="28" t="s">
         <v>178</v>
       </c>
@@ -12985,7 +12710,7 @@
       </c>
       <c r="I155" s="30"/>
     </row>
-    <row r="156" spans="1:9" ht="270">
+    <row r="156" spans="1:9" ht="255">
       <c r="A156" s="28" t="s">
         <v>180</v>
       </c>
@@ -13010,7 +12735,7 @@
       </c>
       <c r="I156" s="30"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9">
       <c r="A157" s="28" t="s">
         <v>181</v>
       </c>
@@ -13035,7 +12760,7 @@
       </c>
       <c r="I157" s="30"/>
     </row>
-    <row r="158" spans="1:9" ht="60">
+    <row r="158" spans="1:9" ht="45">
       <c r="A158" s="28" t="s">
         <v>182</v>
       </c>
@@ -13060,7 +12785,7 @@
       </c>
       <c r="I158" s="30"/>
     </row>
-    <row r="159" spans="1:9" ht="45">
+    <row r="159" spans="1:9" ht="30">
       <c r="A159" s="28" t="s">
         <v>183</v>
       </c>
@@ -13085,7 +12810,7 @@
       </c>
       <c r="I159" s="30"/>
     </row>
-    <row r="160" spans="1:9" ht="45">
+    <row r="160" spans="1:9" ht="30">
       <c r="A160" s="28" t="s">
         <v>184</v>
       </c>
@@ -13110,7 +12835,7 @@
       </c>
       <c r="I160" s="30"/>
     </row>
-    <row r="161" spans="1:9" ht="45">
+    <row r="161" spans="1:9" ht="30">
       <c r="A161" s="28" t="s">
         <v>185</v>
       </c>
@@ -13135,7 +12860,7 @@
       </c>
       <c r="I161" s="30"/>
     </row>
-    <row r="162" spans="1:9" ht="45">
+    <row r="162" spans="1:9" ht="30">
       <c r="A162" s="28" t="s">
         <v>186</v>
       </c>
@@ -13160,7 +12885,7 @@
       </c>
       <c r="I162" s="30"/>
     </row>
-    <row r="163" spans="1:9" ht="270">
+    <row r="163" spans="1:9" ht="180">
       <c r="A163" s="28" t="s">
         <v>187</v>
       </c>
@@ -13187,7 +12912,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9">
       <c r="A164" s="28" t="s">
         <v>188</v>
       </c>
@@ -13214,7 +12939,7 @@
       </c>
       <c r="I164" s="30"/>
     </row>
-    <row r="165" spans="1:9" ht="30">
+    <row r="165" spans="1:9">
       <c r="A165" s="28" t="s">
         <v>189</v>
       </c>
@@ -13241,7 +12966,7 @@
       </c>
       <c r="I165" s="30"/>
     </row>
-    <row r="166" spans="1:9" ht="30">
+    <row r="166" spans="1:9">
       <c r="A166" s="28" t="s">
         <v>190</v>
       </c>
@@ -13268,7 +12993,7 @@
       </c>
       <c r="I166" s="30"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9">
       <c r="A167" s="28" t="s">
         <v>191</v>
       </c>
@@ -13295,7 +13020,7 @@
       </c>
       <c r="I167" s="30"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9">
       <c r="A168" s="28" t="s">
         <v>192</v>
       </c>
@@ -13322,7 +13047,7 @@
       </c>
       <c r="I168" s="30"/>
     </row>
-    <row r="169" spans="1:9" ht="30">
+    <row r="169" spans="1:9">
       <c r="A169" s="28" t="s">
         <v>193</v>
       </c>
@@ -13349,7 +13074,7 @@
       </c>
       <c r="I169" s="30"/>
     </row>
-    <row r="170" spans="1:9" ht="30">
+    <row r="170" spans="1:9">
       <c r="A170" s="28" t="s">
         <v>194</v>
       </c>
@@ -13376,7 +13101,7 @@
       </c>
       <c r="I170" s="30"/>
     </row>
-    <row r="171" spans="1:9" ht="30">
+    <row r="171" spans="1:9">
       <c r="A171" s="28" t="s">
         <v>195</v>
       </c>
@@ -13403,7 +13128,7 @@
       </c>
       <c r="I171" s="30"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9">
       <c r="A172" s="28" t="s">
         <v>196</v>
       </c>
@@ -13430,7 +13155,7 @@
       </c>
       <c r="I172" s="30"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9">
       <c r="A173" s="28" t="s">
         <v>197</v>
       </c>
@@ -13457,7 +13182,7 @@
       </c>
       <c r="I173" s="30"/>
     </row>
-    <row r="174" spans="1:9" ht="30">
+    <row r="174" spans="1:9">
       <c r="A174" s="28" t="s">
         <v>198</v>
       </c>
@@ -13484,7 +13209,7 @@
       </c>
       <c r="I174" s="30"/>
     </row>
-    <row r="175" spans="1:9" ht="30">
+    <row r="175" spans="1:9">
       <c r="A175" s="28" t="s">
         <v>199</v>
       </c>
@@ -13511,7 +13236,7 @@
       </c>
       <c r="I175" s="30"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9">
       <c r="A176" s="28" t="s">
         <v>200</v>
       </c>
@@ -13538,7 +13263,7 @@
       </c>
       <c r="I176" s="30"/>
     </row>
-    <row r="177" spans="1:9" ht="30">
+    <row r="177" spans="1:9">
       <c r="A177" s="28" t="s">
         <v>201</v>
       </c>
@@ -13669,7 +13394,7 @@
       </c>
       <c r="I181" s="33"/>
     </row>
-    <row r="182" spans="1:9" ht="30">
+    <row r="182" spans="1:9">
       <c r="A182" s="28" t="s">
         <v>205</v>
       </c>
@@ -13694,7 +13419,7 @@
       </c>
       <c r="I182" s="30"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9">
       <c r="A183" s="28" t="s">
         <v>206</v>
       </c>
@@ -13719,7 +13444,7 @@
       </c>
       <c r="I183" s="30"/>
     </row>
-    <row r="184" spans="1:9" ht="30">
+    <row r="184" spans="1:9">
       <c r="A184" s="28" t="s">
         <v>207</v>
       </c>
@@ -13819,7 +13544,7 @@
       </c>
       <c r="I187" s="30"/>
     </row>
-    <row r="188" spans="1:9" ht="135">
+    <row r="188" spans="1:9" ht="120">
       <c r="A188" s="28" t="s">
         <v>211</v>
       </c>
@@ -13844,7 +13569,7 @@
       </c>
       <c r="I188" s="30"/>
     </row>
-    <row r="189" spans="1:9" ht="60">
+    <row r="189" spans="1:9" ht="45">
       <c r="A189" s="28" t="s">
         <v>212</v>
       </c>
@@ -14044,7 +13769,7 @@
       </c>
       <c r="I196" s="30"/>
     </row>
-    <row r="197" spans="1:9" ht="45">
+    <row r="197" spans="1:9" ht="30">
       <c r="A197" s="28" t="s">
         <v>219</v>
       </c>
@@ -14069,7 +13794,7 @@
       </c>
       <c r="I197" s="30"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9">
       <c r="A198" s="28" t="s">
         <v>220</v>
       </c>
@@ -14469,7 +14194,7 @@
       </c>
       <c r="I213" s="30"/>
     </row>
-    <row r="214" spans="1:9" ht="60">
+    <row r="214" spans="1:9" ht="45">
       <c r="A214" s="28" t="s">
         <v>236</v>
       </c>
@@ -14496,7 +14221,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="45">
+    <row r="215" spans="1:9" ht="30">
       <c r="A215" s="28" t="s">
         <v>242</v>
       </c>
@@ -14548,7 +14273,7 @@
       </c>
       <c r="I216" s="30"/>
     </row>
-    <row r="217" spans="1:9" ht="45">
+    <row r="217" spans="1:9" ht="30">
       <c r="A217" s="28" t="s">
         <v>244</v>
       </c>
@@ -14598,7 +14323,7 @@
       </c>
       <c r="I218" s="30"/>
     </row>
-    <row r="219" spans="1:9" ht="30">
+    <row r="219" spans="1:9">
       <c r="A219" s="28" t="s">
         <v>246</v>
       </c>
@@ -14648,7 +14373,7 @@
       </c>
       <c r="I220" s="30"/>
     </row>
-    <row r="221" spans="1:9" ht="45">
+    <row r="221" spans="1:9" ht="30">
       <c r="A221" s="28" t="s">
         <v>248</v>
       </c>
@@ -14723,7 +14448,7 @@
       </c>
       <c r="I223" s="30"/>
     </row>
-    <row r="224" spans="1:9" ht="45">
+    <row r="224" spans="1:9" ht="30">
       <c r="A224" s="28" t="s">
         <v>251</v>
       </c>
@@ -14798,7 +14523,7 @@
       </c>
       <c r="I226" s="30"/>
     </row>
-    <row r="227" spans="1:9" ht="30">
+    <row r="227" spans="1:9">
       <c r="A227" s="28" t="s">
         <v>254</v>
       </c>
@@ -15073,7 +14798,7 @@
       </c>
       <c r="I237" s="30"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9">
       <c r="A238" s="28" t="s">
         <v>264</v>
       </c>
@@ -15098,7 +14823,7 @@
       </c>
       <c r="I238" s="30"/>
     </row>
-    <row r="239" spans="1:9" ht="45">
+    <row r="239" spans="1:9" ht="30">
       <c r="A239" s="28" t="s">
         <v>265</v>
       </c>
@@ -15150,7 +14875,7 @@
       </c>
       <c r="I240" s="30"/>
     </row>
-    <row r="241" spans="1:9" ht="45">
+    <row r="241" spans="1:9" ht="30">
       <c r="A241" s="28" t="s">
         <v>267</v>
       </c>
@@ -15200,7 +14925,7 @@
       </c>
       <c r="I242" s="30"/>
     </row>
-    <row r="243" spans="1:9" ht="45">
+    <row r="243" spans="1:9" ht="30">
       <c r="A243" s="28" t="s">
         <v>269</v>
       </c>
@@ -15225,7 +14950,7 @@
       </c>
       <c r="I243" s="30"/>
     </row>
-    <row r="244" spans="1:9" ht="45">
+    <row r="244" spans="1:9" ht="30">
       <c r="A244" s="20" t="s">
         <v>1898</v>
       </c>
@@ -15325,7 +15050,7 @@
       </c>
       <c r="I247" s="30"/>
     </row>
-    <row r="248" spans="1:9" ht="60">
+    <row r="248" spans="1:9" ht="45">
       <c r="A248" s="28" t="s">
         <v>273</v>
       </c>
@@ -15350,7 +15075,7 @@
       </c>
       <c r="I248" s="30"/>
     </row>
-    <row r="249" spans="1:9" ht="75">
+    <row r="249" spans="1:9" ht="60">
       <c r="A249" s="28" t="s">
         <v>274</v>
       </c>
@@ -15400,7 +15125,7 @@
       </c>
       <c r="I250" s="30"/>
     </row>
-    <row r="251" spans="1:9" ht="45">
+    <row r="251" spans="1:9" ht="30">
       <c r="A251" s="28" t="s">
         <v>276</v>
       </c>
@@ -15500,7 +15225,7 @@
       </c>
       <c r="I254" s="30"/>
     </row>
-    <row r="255" spans="1:9" ht="30">
+    <row r="255" spans="1:9">
       <c r="A255" s="28" t="s">
         <v>280</v>
       </c>
@@ -15550,7 +15275,7 @@
       </c>
       <c r="I256" s="30"/>
     </row>
-    <row r="257" spans="1:9" ht="60">
+    <row r="257" spans="1:9" ht="45">
       <c r="A257" s="28" t="s">
         <v>282</v>
       </c>
@@ -15625,7 +15350,7 @@
       </c>
       <c r="I259" s="30"/>
     </row>
-    <row r="260" spans="1:9" ht="150">
+    <row r="260" spans="1:9" ht="135">
       <c r="A260" s="28" t="s">
         <v>285</v>
       </c>
@@ -15650,7 +15375,7 @@
       </c>
       <c r="I260" s="30"/>
     </row>
-    <row r="261" spans="1:9" ht="45">
+    <row r="261" spans="1:9" ht="30">
       <c r="A261" s="28" t="s">
         <v>286</v>
       </c>
@@ -15675,7 +15400,7 @@
       </c>
       <c r="I261" s="30"/>
     </row>
-    <row r="262" spans="1:9" ht="45">
+    <row r="262" spans="1:9" ht="30">
       <c r="A262" s="28" t="s">
         <v>287</v>
       </c>
@@ -15800,7 +15525,7 @@
       </c>
       <c r="I266" s="30"/>
     </row>
-    <row r="267" spans="1:9" ht="45">
+    <row r="267" spans="1:9" ht="30">
       <c r="A267" s="28" t="s">
         <v>292</v>
       </c>
@@ -15825,7 +15550,7 @@
       </c>
       <c r="I267" s="30"/>
     </row>
-    <row r="268" spans="1:9" ht="30">
+    <row r="268" spans="1:9">
       <c r="A268" s="28" t="s">
         <v>293</v>
       </c>
@@ -15925,7 +15650,7 @@
       </c>
       <c r="I271" s="30"/>
     </row>
-    <row r="272" spans="1:9" ht="45">
+    <row r="272" spans="1:9" ht="30">
       <c r="A272" s="28" t="s">
         <v>297</v>
       </c>
@@ -15975,7 +15700,7 @@
       </c>
       <c r="I273" s="30"/>
     </row>
-    <row r="274" spans="1:9" ht="45">
+    <row r="274" spans="1:9" ht="30">
       <c r="A274" s="28" t="s">
         <v>299</v>
       </c>
@@ -16000,7 +15725,7 @@
       </c>
       <c r="I274" s="30"/>
     </row>
-    <row r="275" spans="1:9" ht="30">
+    <row r="275" spans="1:9">
       <c r="A275" s="28" t="s">
         <v>300</v>
       </c>
@@ -16050,7 +15775,7 @@
       </c>
       <c r="I276" s="30"/>
     </row>
-    <row r="277" spans="1:9" ht="30">
+    <row r="277" spans="1:9">
       <c r="A277" s="28" t="s">
         <v>302</v>
       </c>
@@ -16125,7 +15850,7 @@
       </c>
       <c r="I279" s="30"/>
     </row>
-    <row r="280" spans="1:9" ht="60">
+    <row r="280" spans="1:9" ht="45">
       <c r="A280" s="28" t="s">
         <v>305</v>
       </c>
@@ -16175,7 +15900,7 @@
       </c>
       <c r="I281" s="30"/>
     </row>
-    <row r="282" spans="1:9" ht="330">
+    <row r="282" spans="1:9" ht="315">
       <c r="A282" s="28" t="s">
         <v>307</v>
       </c>
@@ -16200,7 +15925,7 @@
       </c>
       <c r="I282" s="30"/>
     </row>
-    <row r="283" spans="1:9" ht="30">
+    <row r="283" spans="1:9">
       <c r="A283" s="28" t="s">
         <v>308</v>
       </c>
@@ -16225,7 +15950,7 @@
       </c>
       <c r="I283" s="30"/>
     </row>
-    <row r="284" spans="1:9" ht="30">
+    <row r="284" spans="1:9">
       <c r="A284" s="28" t="s">
         <v>309</v>
       </c>
@@ -16275,7 +16000,7 @@
       </c>
       <c r="I285" s="30"/>
     </row>
-    <row r="286" spans="1:9" ht="30">
+    <row r="286" spans="1:9">
       <c r="A286" s="28" t="s">
         <v>311</v>
       </c>
@@ -16350,7 +16075,7 @@
       </c>
       <c r="I288" s="30"/>
     </row>
-    <row r="289" spans="1:9" ht="30">
+    <row r="289" spans="1:9">
       <c r="A289" s="28" t="s">
         <v>314</v>
       </c>
@@ -16375,7 +16100,7 @@
       </c>
       <c r="I289" s="30"/>
     </row>
-    <row r="290" spans="1:9" ht="30">
+    <row r="290" spans="1:9">
       <c r="A290" s="28" t="s">
         <v>315</v>
       </c>
@@ -16875,7 +16600,7 @@
       </c>
       <c r="I309" s="30"/>
     </row>
-    <row r="310" spans="1:9" ht="75">
+    <row r="310" spans="1:9" ht="60">
       <c r="A310" s="28" t="s">
         <v>335</v>
       </c>
@@ -16900,7 +16625,7 @@
       </c>
       <c r="I310" s="30"/>
     </row>
-    <row r="311" spans="1:9" ht="345">
+    <row r="311" spans="1:9" ht="330">
       <c r="A311" s="28" t="s">
         <v>336</v>
       </c>
@@ -16925,7 +16650,7 @@
       </c>
       <c r="I311" s="30"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9">
       <c r="A312" s="28" t="s">
         <v>337</v>
       </c>
@@ -16950,7 +16675,7 @@
       </c>
       <c r="I312" s="30"/>
     </row>
-    <row r="313" spans="1:9" ht="30">
+    <row r="313" spans="1:9">
       <c r="A313" s="28" t="s">
         <v>338</v>
       </c>
@@ -17125,7 +16850,7 @@
       </c>
       <c r="I319" s="30"/>
     </row>
-    <row r="320" spans="1:9" ht="30">
+    <row r="320" spans="1:9">
       <c r="A320" s="28" t="s">
         <v>345</v>
       </c>
@@ -17150,7 +16875,7 @@
       </c>
       <c r="I320" s="30"/>
     </row>
-    <row r="321" spans="1:9" ht="30">
+    <row r="321" spans="1:9">
       <c r="A321" s="28" t="s">
         <v>346</v>
       </c>
@@ -17275,7 +17000,7 @@
       </c>
       <c r="I325" s="30"/>
     </row>
-    <row r="326" spans="1:9" ht="30">
+    <row r="326" spans="1:9">
       <c r="A326" s="28" t="s">
         <v>351</v>
       </c>
@@ -17350,7 +17075,7 @@
       </c>
       <c r="I328" s="30"/>
     </row>
-    <row r="329" spans="1:9" ht="30">
+    <row r="329" spans="1:9">
       <c r="A329" s="28" t="s">
         <v>354</v>
       </c>
@@ -17500,7 +17225,7 @@
       </c>
       <c r="I334" s="30"/>
     </row>
-    <row r="335" spans="1:9" ht="30">
+    <row r="335" spans="1:9">
       <c r="A335" s="28" t="s">
         <v>360</v>
       </c>
@@ -17625,7 +17350,7 @@
       </c>
       <c r="I339" s="30"/>
     </row>
-    <row r="340" spans="1:9" ht="30">
+    <row r="340" spans="1:9">
       <c r="A340" s="28" t="s">
         <v>364</v>
       </c>
@@ -17650,7 +17375,7 @@
       </c>
       <c r="I340" s="30"/>
     </row>
-    <row r="341" spans="1:9" ht="30">
+    <row r="341" spans="1:9">
       <c r="A341" s="28" t="s">
         <v>365</v>
       </c>
@@ -17700,7 +17425,7 @@
       </c>
       <c r="I342" s="30"/>
     </row>
-    <row r="343" spans="1:9" ht="45">
+    <row r="343" spans="1:9" ht="30">
       <c r="A343" s="28" t="s">
         <v>367</v>
       </c>
@@ -17775,7 +17500,7 @@
       </c>
       <c r="I345" s="30"/>
     </row>
-    <row r="346" spans="1:9" ht="45">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="28" t="s">
         <v>370</v>
       </c>
@@ -17825,7 +17550,7 @@
       </c>
       <c r="I347" s="30"/>
     </row>
-    <row r="348" spans="1:9" ht="45">
+    <row r="348" spans="1:9" ht="30">
       <c r="A348" s="28" t="s">
         <v>372</v>
       </c>
@@ -17875,7 +17600,7 @@
       </c>
       <c r="I349" s="30"/>
     </row>
-    <row r="350" spans="1:9" ht="45">
+    <row r="350" spans="1:9" ht="30">
       <c r="A350" s="28" t="s">
         <v>374</v>
       </c>
@@ -17900,7 +17625,7 @@
       </c>
       <c r="I350" s="30"/>
     </row>
-    <row r="351" spans="1:9" ht="45">
+    <row r="351" spans="1:9" ht="30">
       <c r="A351" s="28" t="s">
         <v>375</v>
       </c>
@@ -17950,7 +17675,7 @@
       </c>
       <c r="I352" s="30"/>
     </row>
-    <row r="353" spans="1:9" ht="75">
+    <row r="353" spans="1:9" ht="45">
       <c r="A353" s="28" t="s">
         <v>377</v>
       </c>
@@ -18000,7 +17725,7 @@
       </c>
       <c r="I354" s="30"/>
     </row>
-    <row r="355" spans="1:9" ht="30">
+    <row r="355" spans="1:9">
       <c r="A355" s="28" t="s">
         <v>379</v>
       </c>
@@ -18025,7 +17750,7 @@
       </c>
       <c r="I355" s="30"/>
     </row>
-    <row r="356" spans="1:9" ht="45">
+    <row r="356" spans="1:9" ht="30">
       <c r="A356" s="28" t="s">
         <v>380</v>
       </c>
@@ -18150,7 +17875,7 @@
       </c>
       <c r="I360" s="30"/>
     </row>
-    <row r="361" spans="1:9" ht="45">
+    <row r="361" spans="1:9" ht="30">
       <c r="A361" s="28" t="s">
         <v>385</v>
       </c>
@@ -18250,7 +17975,7 @@
       </c>
       <c r="I364" s="30"/>
     </row>
-    <row r="365" spans="1:9" ht="30">
+    <row r="365" spans="1:9">
       <c r="A365" s="28" t="s">
         <v>389</v>
       </c>
@@ -18275,7 +18000,7 @@
       </c>
       <c r="I365" s="30"/>
     </row>
-    <row r="366" spans="1:9" ht="45">
+    <row r="366" spans="1:9" ht="30">
       <c r="A366" s="28" t="s">
         <v>390</v>
       </c>
@@ -18325,7 +18050,7 @@
       </c>
       <c r="I367" s="30"/>
     </row>
-    <row r="368" spans="1:9" ht="30">
+    <row r="368" spans="1:9">
       <c r="A368" s="28" t="s">
         <v>392</v>
       </c>
@@ -18450,7 +18175,7 @@
       </c>
       <c r="I372" s="30"/>
     </row>
-    <row r="373" spans="1:9" ht="45">
+    <row r="373" spans="1:9" ht="30">
       <c r="A373" s="28" t="s">
         <v>397</v>
       </c>
@@ -18702,7 +18427,7 @@
       </c>
       <c r="I382" s="30"/>
     </row>
-    <row r="383" spans="1:9" ht="30">
+    <row r="383" spans="1:9">
       <c r="A383" s="28" t="s">
         <v>407</v>
       </c>
@@ -18752,7 +18477,7 @@
       </c>
       <c r="I384" s="30"/>
     </row>
-    <row r="385" spans="1:9" ht="30">
+    <row r="385" spans="1:9">
       <c r="A385" s="28" t="s">
         <v>409</v>
       </c>
@@ -18802,7 +18527,7 @@
       </c>
       <c r="I386" s="30"/>
     </row>
-    <row r="387" spans="1:9" ht="30">
+    <row r="387" spans="1:9">
       <c r="A387" s="28" t="s">
         <v>411</v>
       </c>
@@ -18902,7 +18627,7 @@
       </c>
       <c r="I390" s="30"/>
     </row>
-    <row r="391" spans="1:9" ht="30">
+    <row r="391" spans="1:9">
       <c r="A391" s="28" t="s">
         <v>415</v>
       </c>
@@ -19002,7 +18727,7 @@
       </c>
       <c r="I394" s="30"/>
     </row>
-    <row r="395" spans="1:9" ht="45">
+    <row r="395" spans="1:9" ht="30">
       <c r="A395" s="28" t="s">
         <v>419</v>
       </c>
@@ -19027,7 +18752,7 @@
       </c>
       <c r="I395" s="30"/>
     </row>
-    <row r="396" spans="1:9" ht="45">
+    <row r="396" spans="1:9" ht="30">
       <c r="A396" s="28" t="s">
         <v>420</v>
       </c>
@@ -19077,7 +18802,7 @@
       </c>
       <c r="I397" s="30"/>
     </row>
-    <row r="398" spans="1:9" ht="45">
+    <row r="398" spans="1:9" ht="30">
       <c r="A398" s="28" t="s">
         <v>422</v>
       </c>
@@ -19152,7 +18877,7 @@
       </c>
       <c r="I400" s="30"/>
     </row>
-    <row r="401" spans="1:9" ht="45">
+    <row r="401" spans="1:9" ht="30">
       <c r="A401" s="28" t="s">
         <v>425</v>
       </c>
@@ -19252,7 +18977,7 @@
       </c>
       <c r="I404" s="18"/>
     </row>
-    <row r="405" spans="1:9" ht="45">
+    <row r="405" spans="1:9" ht="30">
       <c r="A405" s="28" t="s">
         <v>429</v>
       </c>
@@ -19279,7 +19004,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="406" spans="1:9" ht="90">
+    <row r="406" spans="1:9" ht="75">
       <c r="A406" s="28" t="s">
         <v>430</v>
       </c>
@@ -19354,7 +19079,7 @@
       </c>
       <c r="I408" s="30"/>
     </row>
-    <row r="409" spans="1:9" ht="45">
+    <row r="409" spans="1:9" ht="30">
       <c r="A409" s="28" t="s">
         <v>433</v>
       </c>
@@ -19579,7 +19304,7 @@
       </c>
       <c r="I417" s="30"/>
     </row>
-    <row r="418" spans="1:9" ht="45">
+    <row r="418" spans="1:9" ht="30">
       <c r="A418" s="28" t="s">
         <v>442</v>
       </c>
@@ -19679,7 +19404,7 @@
       </c>
       <c r="I421" s="30"/>
     </row>
-    <row r="422" spans="1:9" ht="45">
+    <row r="422" spans="1:9" ht="30">
       <c r="A422" s="28" t="s">
         <v>446</v>
       </c>
@@ -19729,7 +19454,7 @@
       </c>
       <c r="I423" s="30"/>
     </row>
-    <row r="424" spans="1:9" ht="45">
+    <row r="424" spans="1:9" ht="30">
       <c r="A424" s="28" t="s">
         <v>448</v>
       </c>
@@ -19754,7 +19479,7 @@
       </c>
       <c r="I424" s="30"/>
     </row>
-    <row r="425" spans="1:9" ht="30">
+    <row r="425" spans="1:9">
       <c r="A425" s="28" t="s">
         <v>449</v>
       </c>
@@ -19879,7 +19604,7 @@
       </c>
       <c r="I429" s="30"/>
     </row>
-    <row r="430" spans="1:9" ht="60">
+    <row r="430" spans="1:9" ht="45">
       <c r="A430" s="28" t="s">
         <v>454</v>
       </c>
@@ -19904,7 +19629,7 @@
       </c>
       <c r="I430" s="30"/>
     </row>
-    <row r="431" spans="1:9" ht="135">
+    <row r="431" spans="1:9" ht="120">
       <c r="A431" s="28" t="s">
         <v>455</v>
       </c>
@@ -19954,7 +19679,7 @@
       </c>
       <c r="I432" s="30"/>
     </row>
-    <row r="433" spans="1:9" ht="150">
+    <row r="433" spans="1:9" ht="135">
       <c r="A433" s="28" t="s">
         <v>457</v>
       </c>
@@ -20004,7 +19729,7 @@
       </c>
       <c r="I434" s="30"/>
     </row>
-    <row r="435" spans="1:9" ht="75">
+    <row r="435" spans="1:9" ht="60">
       <c r="A435" s="28" t="s">
         <v>459</v>
       </c>
@@ -20081,7 +19806,7 @@
       </c>
       <c r="I437" s="30"/>
     </row>
-    <row r="438" spans="1:9" ht="60">
+    <row r="438" spans="1:9" ht="45">
       <c r="A438" s="28" t="s">
         <v>463</v>
       </c>
@@ -20106,7 +19831,7 @@
       </c>
       <c r="I438" s="30"/>
     </row>
-    <row r="439" spans="1:9" ht="45">
+    <row r="439" spans="1:9" ht="30">
       <c r="A439" s="28" t="s">
         <v>464</v>
       </c>
@@ -20206,7 +19931,7 @@
       </c>
       <c r="I442" s="30"/>
     </row>
-    <row r="443" spans="1:9" ht="30">
+    <row r="443" spans="1:9">
       <c r="A443" s="28" t="s">
         <v>468</v>
       </c>
@@ -20252,7 +19977,7 @@
         <v>15</v>
       </c>
       <c r="H444" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I444" s="30"/>
     </row>
@@ -20277,7 +20002,7 @@
         <v>15</v>
       </c>
       <c r="H445" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I445" s="30"/>
     </row>
@@ -20331,7 +20056,7 @@
       </c>
       <c r="I447" s="30"/>
     </row>
-    <row r="448" spans="1:9" ht="45">
+    <row r="448" spans="1:9" ht="30">
       <c r="A448" s="28" t="s">
         <v>473</v>
       </c>
@@ -20356,7 +20081,7 @@
       </c>
       <c r="I448" s="30"/>
     </row>
-    <row r="449" spans="1:9" ht="60">
+    <row r="449" spans="1:9" ht="45">
       <c r="A449" s="28" t="s">
         <v>474</v>
       </c>
@@ -20456,7 +20181,7 @@
       </c>
       <c r="I452" s="30"/>
     </row>
-    <row r="453" spans="1:9" ht="45">
+    <row r="453" spans="1:9" ht="30">
       <c r="A453" s="28" t="s">
         <v>478</v>
       </c>
@@ -20881,7 +20606,7 @@
       </c>
       <c r="I469" s="30"/>
     </row>
-    <row r="470" spans="1:9" ht="255">
+    <row r="470" spans="1:9" ht="240">
       <c r="A470" s="28" t="s">
         <v>495</v>
       </c>
@@ -20931,7 +20656,7 @@
       </c>
       <c r="I471" s="30"/>
     </row>
-    <row r="472" spans="1:9" ht="120">
+    <row r="472" spans="1:9" ht="105">
       <c r="A472" s="28" t="s">
         <v>497</v>
       </c>
@@ -20956,7 +20681,7 @@
       </c>
       <c r="I472" s="30"/>
     </row>
-    <row r="473" spans="1:9" ht="45">
+    <row r="473" spans="1:9" ht="30">
       <c r="A473" s="28" t="s">
         <v>498</v>
       </c>
@@ -21008,7 +20733,7 @@
       </c>
       <c r="I474" s="30"/>
     </row>
-    <row r="475" spans="1:9" ht="45">
+    <row r="475" spans="1:9" ht="30">
       <c r="A475" s="28" t="s">
         <v>500</v>
       </c>
@@ -21033,7 +20758,7 @@
       </c>
       <c r="I475" s="30"/>
     </row>
-    <row r="476" spans="1:9" ht="30">
+    <row r="476" spans="1:9">
       <c r="A476" s="28" t="s">
         <v>501</v>
       </c>
@@ -21058,7 +20783,7 @@
       </c>
       <c r="I476" s="30"/>
     </row>
-    <row r="477" spans="1:9" ht="30">
+    <row r="477" spans="1:9">
       <c r="A477" s="28" t="s">
         <v>502</v>
       </c>
@@ -21158,7 +20883,7 @@
       </c>
       <c r="I480" s="30"/>
     </row>
-    <row r="481" spans="1:9" ht="60">
+    <row r="481" spans="1:9" ht="45">
       <c r="A481" s="28" t="s">
         <v>506</v>
       </c>
@@ -21283,7 +21008,7 @@
       </c>
       <c r="I485" s="30"/>
     </row>
-    <row r="486" spans="1:9" ht="30">
+    <row r="486" spans="1:9">
       <c r="A486" s="28" t="s">
         <v>511</v>
       </c>
@@ -21333,7 +21058,7 @@
       </c>
       <c r="I487" s="30"/>
     </row>
-    <row r="488" spans="1:9" ht="45">
+    <row r="488" spans="1:9" ht="30">
       <c r="A488" s="28" t="s">
         <v>513</v>
       </c>
@@ -21433,7 +21158,7 @@
       </c>
       <c r="I491" s="30"/>
     </row>
-    <row r="492" spans="1:9" ht="30">
+    <row r="492" spans="1:9">
       <c r="A492" s="28" t="s">
         <v>517</v>
       </c>
@@ -21508,7 +21233,7 @@
       </c>
       <c r="I494" s="30"/>
     </row>
-    <row r="495" spans="1:9" ht="45">
+    <row r="495" spans="1:9" ht="30">
       <c r="A495" s="28" t="s">
         <v>520</v>
       </c>
@@ -21533,7 +21258,7 @@
       </c>
       <c r="I495" s="30"/>
     </row>
-    <row r="496" spans="1:9" ht="30">
+    <row r="496" spans="1:9">
       <c r="A496" s="28" t="s">
         <v>521</v>
       </c>
@@ -21608,7 +21333,7 @@
       </c>
       <c r="I498" s="33"/>
     </row>
-    <row r="499" spans="1:9" ht="45">
+    <row r="499" spans="1:9" ht="30">
       <c r="A499" s="20" t="s">
         <v>523</v>
       </c>
@@ -21820,7 +21545,7 @@
       </c>
       <c r="I506" s="30"/>
     </row>
-    <row r="507" spans="1:9" ht="60">
+    <row r="507" spans="1:9" ht="45">
       <c r="A507" s="28" t="s">
         <v>528</v>
       </c>
@@ -22007,7 +21732,7 @@
       </c>
       <c r="I513" s="30"/>
     </row>
-    <row r="514" spans="1:9" ht="30">
+    <row r="514" spans="1:9">
       <c r="A514" s="28" t="s">
         <v>532</v>
       </c>
@@ -22182,7 +21907,7 @@
       </c>
       <c r="I520" s="30"/>
     </row>
-    <row r="521" spans="1:9" ht="30">
+    <row r="521" spans="1:9">
       <c r="A521" s="28" t="s">
         <v>540</v>
       </c>
@@ -22357,7 +22082,7 @@
       </c>
       <c r="I527" s="30"/>
     </row>
-    <row r="528" spans="1:9" ht="30">
+    <row r="528" spans="1:9">
       <c r="A528" s="28" t="s">
         <v>547</v>
       </c>
@@ -22432,7 +22157,7 @@
       </c>
       <c r="I530" s="30"/>
     </row>
-    <row r="531" spans="1:9" ht="45">
+    <row r="531" spans="1:9" ht="30">
       <c r="A531" s="28" t="s">
         <v>550</v>
       </c>
@@ -22582,7 +22307,7 @@
       </c>
       <c r="I536" s="30"/>
     </row>
-    <row r="537" spans="1:9" ht="60">
+    <row r="537" spans="1:9" ht="45">
       <c r="A537" s="28" t="s">
         <v>556</v>
       </c>
@@ -22632,7 +22357,7 @@
       </c>
       <c r="I538" s="30"/>
     </row>
-    <row r="539" spans="1:9" ht="135">
+    <row r="539" spans="1:9" ht="120">
       <c r="A539" s="28" t="s">
         <v>558</v>
       </c>
@@ -22782,7 +22507,7 @@
       </c>
       <c r="I544" s="30"/>
     </row>
-    <row r="545" spans="1:9" ht="30">
+    <row r="545" spans="1:9">
       <c r="A545" s="28" t="s">
         <v>564</v>
       </c>
@@ -22807,7 +22532,7 @@
       </c>
       <c r="I545" s="30"/>
     </row>
-    <row r="546" spans="1:9" ht="60">
+    <row r="546" spans="1:9" ht="45">
       <c r="A546" s="28" t="s">
         <v>565</v>
       </c>
@@ -22911,7 +22636,7 @@
       </c>
       <c r="I549" s="30"/>
     </row>
-    <row r="550" spans="1:9" ht="45">
+    <row r="550" spans="1:9" ht="30">
       <c r="A550" s="28" t="s">
         <v>571</v>
       </c>
@@ -22936,7 +22661,7 @@
       </c>
       <c r="I550" s="30"/>
     </row>
-    <row r="551" spans="1:9" ht="30">
+    <row r="551" spans="1:9">
       <c r="A551" s="28" t="s">
         <v>572</v>
       </c>
@@ -23036,7 +22761,7 @@
       </c>
       <c r="I554" s="30"/>
     </row>
-    <row r="555" spans="1:9" ht="45">
+    <row r="555" spans="1:9" ht="30">
       <c r="A555" s="28" t="s">
         <v>576</v>
       </c>
@@ -23061,7 +22786,7 @@
       </c>
       <c r="I555" s="30"/>
     </row>
-    <row r="556" spans="1:9" ht="45">
+    <row r="556" spans="1:9" ht="30">
       <c r="A556" s="28" t="s">
         <v>577</v>
       </c>
@@ -23186,7 +22911,7 @@
       </c>
       <c r="I560" s="30"/>
     </row>
-    <row r="561" spans="1:9" ht="30">
+    <row r="561" spans="1:9">
       <c r="A561" s="28" t="s">
         <v>582</v>
       </c>
@@ -23236,7 +22961,7 @@
       </c>
       <c r="I562" s="30"/>
     </row>
-    <row r="563" spans="1:9" ht="45">
+    <row r="563" spans="1:9" ht="30">
       <c r="A563" s="28" t="s">
         <v>584</v>
       </c>
@@ -23311,7 +23036,7 @@
       </c>
       <c r="I565" s="30"/>
     </row>
-    <row r="566" spans="1:9" ht="345">
+    <row r="566" spans="1:9" ht="330">
       <c r="A566" s="28" t="s">
         <v>587</v>
       </c>
@@ -23336,7 +23061,7 @@
       </c>
       <c r="I566" s="30"/>
     </row>
-    <row r="567" spans="1:9" ht="30">
+    <row r="567" spans="1:9">
       <c r="A567" s="28" t="s">
         <v>588</v>
       </c>
@@ -23411,7 +23136,7 @@
       </c>
       <c r="I569" s="30"/>
     </row>
-    <row r="570" spans="1:9" ht="30">
+    <row r="570" spans="1:9">
       <c r="A570" s="28" t="s">
         <v>591</v>
       </c>
@@ -23461,7 +23186,7 @@
       </c>
       <c r="I571" s="30"/>
     </row>
-    <row r="572" spans="1:9" ht="45">
+    <row r="572" spans="1:9" ht="30">
       <c r="A572" s="28" t="s">
         <v>593</v>
       </c>
@@ -23588,7 +23313,7 @@
       </c>
       <c r="I576" s="30"/>
     </row>
-    <row r="577" spans="1:9" ht="45">
+    <row r="577" spans="1:9" ht="30">
       <c r="A577" s="28" t="s">
         <v>598</v>
       </c>
@@ -23663,7 +23388,7 @@
       </c>
       <c r="I579" s="30"/>
     </row>
-    <row r="580" spans="1:9" ht="60">
+    <row r="580" spans="1:9" ht="45">
       <c r="A580" s="28" t="s">
         <v>601</v>
       </c>
@@ -23713,7 +23438,7 @@
       </c>
       <c r="I581" s="30"/>
     </row>
-    <row r="582" spans="1:9" ht="45">
+    <row r="582" spans="1:9" ht="30">
       <c r="A582" s="28" t="s">
         <v>603</v>
       </c>
@@ -23813,7 +23538,7 @@
       </c>
       <c r="I585" s="30"/>
     </row>
-    <row r="586" spans="1:9" ht="45">
+    <row r="586" spans="1:9" ht="30">
       <c r="A586" s="28" t="s">
         <v>607</v>
       </c>
@@ -23988,7 +23713,7 @@
       </c>
       <c r="I592" s="30"/>
     </row>
-    <row r="593" spans="1:9" ht="45">
+    <row r="593" spans="1:9" ht="30">
       <c r="A593" s="28" t="s">
         <v>613</v>
       </c>
@@ -24063,7 +23788,7 @@
       </c>
       <c r="I595" s="30"/>
     </row>
-    <row r="596" spans="1:9" ht="30">
+    <row r="596" spans="1:9">
       <c r="A596" s="28" t="s">
         <v>616</v>
       </c>
@@ -24088,7 +23813,7 @@
       </c>
       <c r="I596" s="30"/>
     </row>
-    <row r="597" spans="1:9" ht="45">
+    <row r="597" spans="1:9" ht="30">
       <c r="A597" s="28" t="s">
         <v>617</v>
       </c>
@@ -24115,7 +23840,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="598" spans="1:9" ht="90">
+    <row r="598" spans="1:9" ht="75">
       <c r="A598" s="28" t="s">
         <v>618</v>
       </c>
@@ -24140,7 +23865,7 @@
       </c>
       <c r="I598" s="30"/>
     </row>
-    <row r="599" spans="1:9" ht="45">
+    <row r="599" spans="1:9" ht="30">
       <c r="A599" s="28" t="s">
         <v>619</v>
       </c>
@@ -24290,7 +24015,7 @@
       </c>
       <c r="I604" s="30"/>
     </row>
-    <row r="605" spans="1:9" ht="45">
+    <row r="605" spans="1:9" ht="30">
       <c r="A605" s="28" t="s">
         <v>625</v>
       </c>
@@ -24340,7 +24065,7 @@
       </c>
       <c r="I606" s="30"/>
     </row>
-    <row r="607" spans="1:9" ht="45">
+    <row r="607" spans="1:9" ht="30">
       <c r="A607" s="28" t="s">
         <v>627</v>
       </c>
@@ -24390,7 +24115,7 @@
       </c>
       <c r="I608" s="30"/>
     </row>
-    <row r="609" spans="1:9" ht="45">
+    <row r="609" spans="1:9" ht="30">
       <c r="A609" s="28" t="s">
         <v>629</v>
       </c>
@@ -24490,7 +24215,7 @@
       </c>
       <c r="I612" s="30"/>
     </row>
-    <row r="613" spans="1:9" ht="45">
+    <row r="613" spans="1:9" ht="30">
       <c r="A613" s="28" t="s">
         <v>633</v>
       </c>
@@ -24565,7 +24290,7 @@
       </c>
       <c r="I615" s="30"/>
     </row>
-    <row r="616" spans="1:9" ht="45">
+    <row r="616" spans="1:9" ht="30">
       <c r="A616" s="28" t="s">
         <v>636</v>
       </c>
@@ -24692,7 +24417,7 @@
       </c>
       <c r="I620" s="30"/>
     </row>
-    <row r="621" spans="1:9" ht="45">
+    <row r="621" spans="1:9" ht="30">
       <c r="A621" s="28" t="s">
         <v>641</v>
       </c>
@@ -24717,7 +24442,7 @@
       </c>
       <c r="I621" s="30"/>
     </row>
-    <row r="622" spans="1:9" ht="45">
+    <row r="622" spans="1:9" ht="30">
       <c r="A622" s="28" t="s">
         <v>642</v>
       </c>
@@ -24892,7 +24617,7 @@
       </c>
       <c r="I628" s="30"/>
     </row>
-    <row r="629" spans="1:9" ht="60">
+    <row r="629" spans="1:9" ht="45">
       <c r="A629" s="28" t="s">
         <v>649</v>
       </c>
@@ -25017,7 +24742,7 @@
       </c>
       <c r="I633" s="30"/>
     </row>
-    <row r="634" spans="1:9" ht="45">
+    <row r="634" spans="1:9" ht="30">
       <c r="A634" s="28" t="s">
         <v>654</v>
       </c>
@@ -25042,7 +24767,7 @@
       </c>
       <c r="I634" s="30"/>
     </row>
-    <row r="635" spans="1:9" ht="45">
+    <row r="635" spans="1:9" ht="30">
       <c r="A635" s="28" t="s">
         <v>655</v>
       </c>
@@ -25142,7 +24867,7 @@
       </c>
       <c r="I638" s="30"/>
     </row>
-    <row r="639" spans="1:9" ht="75">
+    <row r="639" spans="1:9" ht="60">
       <c r="A639" s="28" t="s">
         <v>659</v>
       </c>
@@ -25169,7 +24894,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="640" spans="1:9" ht="45">
+    <row r="640" spans="1:9" ht="30">
       <c r="A640" s="28" t="s">
         <v>661</v>
       </c>
@@ -25196,7 +24921,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="641" spans="1:9" ht="90">
+    <row r="641" spans="1:9" ht="75">
       <c r="A641" s="28" t="s">
         <v>662</v>
       </c>
@@ -25221,7 +24946,7 @@
       </c>
       <c r="I641" s="30"/>
     </row>
-    <row r="642" spans="1:9" ht="45">
+    <row r="642" spans="1:9" ht="30">
       <c r="A642" s="28" t="s">
         <v>663</v>
       </c>
@@ -25246,7 +24971,7 @@
       </c>
       <c r="I642" s="30"/>
     </row>
-    <row r="643" spans="1:9" ht="30">
+    <row r="643" spans="1:9">
       <c r="A643" s="28" t="s">
         <v>664</v>
       </c>
@@ -25346,7 +25071,7 @@
       </c>
       <c r="I646" s="30"/>
     </row>
-    <row r="647" spans="1:9" ht="45">
+    <row r="647" spans="1:9" ht="30">
       <c r="A647" s="28" t="s">
         <v>668</v>
       </c>
@@ -25471,7 +25196,7 @@
       </c>
       <c r="I651" s="30"/>
     </row>
-    <row r="652" spans="1:9" ht="45">
+    <row r="652" spans="1:9" ht="30">
       <c r="A652" s="28" t="s">
         <v>673</v>
       </c>
@@ -25496,7 +25221,7 @@
       </c>
       <c r="I652" s="30"/>
     </row>
-    <row r="653" spans="1:9" ht="30">
+    <row r="653" spans="1:9">
       <c r="A653" s="28" t="s">
         <v>674</v>
       </c>
@@ -25521,7 +25246,7 @@
       </c>
       <c r="I653" s="30"/>
     </row>
-    <row r="654" spans="1:9" ht="45">
+    <row r="654" spans="1:9" ht="30">
       <c r="A654" s="28" t="s">
         <v>675</v>
       </c>
@@ -25746,7 +25471,7 @@
       </c>
       <c r="I662" s="30"/>
     </row>
-    <row r="663" spans="1:9" ht="60">
+    <row r="663" spans="1:9" ht="45">
       <c r="A663" s="28" t="s">
         <v>684</v>
       </c>
@@ -25796,7 +25521,7 @@
       </c>
       <c r="I664" s="30"/>
     </row>
-    <row r="665" spans="1:9" ht="60">
+    <row r="665" spans="1:9" ht="45">
       <c r="A665" s="28" t="s">
         <v>686</v>
       </c>
@@ -25821,7 +25546,7 @@
       </c>
       <c r="I665" s="30"/>
     </row>
-    <row r="666" spans="1:9" ht="105">
+    <row r="666" spans="1:9" ht="90">
       <c r="A666" s="28" t="s">
         <v>687</v>
       </c>
@@ -25875,7 +25600,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="668" spans="1:9" ht="45">
+    <row r="668" spans="1:9" ht="30">
       <c r="A668" s="28" t="s">
         <v>693</v>
       </c>
@@ -25900,7 +25625,7 @@
       </c>
       <c r="I668" s="30"/>
     </row>
-    <row r="669" spans="1:9" ht="45">
+    <row r="669" spans="1:9" ht="30">
       <c r="A669" s="28" t="s">
         <v>694</v>
       </c>
@@ -26000,7 +25725,7 @@
       </c>
       <c r="I672" s="30"/>
     </row>
-    <row r="673" spans="1:9" ht="30">
+    <row r="673" spans="1:9">
       <c r="A673" s="28" t="s">
         <v>698</v>
       </c>
@@ -26025,7 +25750,7 @@
       </c>
       <c r="I673" s="30"/>
     </row>
-    <row r="674" spans="1:9" ht="30">
+    <row r="674" spans="1:9">
       <c r="A674" s="28" t="s">
         <v>699</v>
       </c>
@@ -26125,7 +25850,7 @@
       </c>
       <c r="I677" s="30"/>
     </row>
-    <row r="678" spans="1:9" ht="45">
+    <row r="678" spans="1:9" ht="30">
       <c r="A678" s="28" t="s">
         <v>703</v>
       </c>
@@ -26350,7 +26075,7 @@
       </c>
       <c r="I686" s="30"/>
     </row>
-    <row r="687" spans="1:9" ht="60">
+    <row r="687" spans="1:9" ht="45">
       <c r="A687" s="28" t="s">
         <v>712</v>
       </c>
@@ -26475,7 +26200,7 @@
       </c>
       <c r="I691" s="30"/>
     </row>
-    <row r="692" spans="1:9" ht="45">
+    <row r="692" spans="1:9" ht="30">
       <c r="A692" s="28" t="s">
         <v>717</v>
       </c>
@@ -26500,7 +26225,7 @@
       </c>
       <c r="I692" s="30"/>
     </row>
-    <row r="693" spans="1:9" ht="45">
+    <row r="693" spans="1:9" ht="30">
       <c r="A693" s="28" t="s">
         <v>718</v>
       </c>
@@ -26525,7 +26250,7 @@
       </c>
       <c r="I693" s="30"/>
     </row>
-    <row r="694" spans="1:9" ht="45">
+    <row r="694" spans="1:9" ht="30">
       <c r="A694" s="28" t="s">
         <v>719</v>
       </c>
@@ -27000,7 +26725,7 @@
       </c>
       <c r="I712" s="30"/>
     </row>
-    <row r="713" spans="1:9" ht="45">
+    <row r="713" spans="1:9" ht="30">
       <c r="A713" s="28" t="s">
         <v>737</v>
       </c>
@@ -27225,7 +26950,7 @@
       </c>
       <c r="I721" s="30"/>
     </row>
-    <row r="722" spans="1:9" ht="30">
+    <row r="722" spans="1:9">
       <c r="A722" s="28" t="s">
         <v>741</v>
       </c>
@@ -27750,7 +27475,7 @@
       </c>
       <c r="I742" s="30"/>
     </row>
-    <row r="743" spans="1:9" ht="105">
+    <row r="743" spans="1:9" ht="75">
       <c r="A743" s="28" t="s">
         <v>761</v>
       </c>
@@ -27802,7 +27527,7 @@
       </c>
       <c r="I744" s="30"/>
     </row>
-    <row r="745" spans="1:9" ht="75">
+    <row r="745" spans="1:9" ht="60">
       <c r="A745" s="28" t="s">
         <v>763</v>
       </c>
@@ -27827,7 +27552,7 @@
       </c>
       <c r="I745" s="30"/>
     </row>
-    <row r="746" spans="1:9" ht="75">
+    <row r="746" spans="1:9" ht="60">
       <c r="A746" s="28" t="s">
         <v>764</v>
       </c>
@@ -27877,7 +27602,7 @@
       </c>
       <c r="I747" s="30"/>
     </row>
-    <row r="748" spans="1:9" ht="45">
+    <row r="748" spans="1:9" ht="30">
       <c r="A748" s="28" t="s">
         <v>771</v>
       </c>
@@ -27929,7 +27654,7 @@
       </c>
       <c r="I749" s="30"/>
     </row>
-    <row r="750" spans="1:9" ht="45">
+    <row r="750" spans="1:9" ht="30">
       <c r="A750" s="28" t="s">
         <v>773</v>
       </c>
@@ -27954,7 +27679,7 @@
       </c>
       <c r="I750" s="30"/>
     </row>
-    <row r="751" spans="1:9" ht="30">
+    <row r="751" spans="1:9">
       <c r="A751" s="28" t="s">
         <v>774</v>
       </c>
@@ -28079,7 +27804,7 @@
       </c>
       <c r="I755" s="18"/>
     </row>
-    <row r="756" spans="1:9" ht="30">
+    <row r="756" spans="1:9">
       <c r="A756" s="28" t="s">
         <v>779</v>
       </c>
@@ -28104,7 +27829,7 @@
       </c>
       <c r="I756" s="30"/>
     </row>
-    <row r="757" spans="1:9" ht="30">
+    <row r="757" spans="1:9">
       <c r="A757" s="28" t="s">
         <v>780</v>
       </c>
@@ -28129,7 +27854,7 @@
       </c>
       <c r="I757" s="30"/>
     </row>
-    <row r="758" spans="1:9" ht="30">
+    <row r="758" spans="1:9">
       <c r="A758" s="28" t="s">
         <v>781</v>
       </c>
@@ -28154,7 +27879,7 @@
       </c>
       <c r="I758" s="30"/>
     </row>
-    <row r="759" spans="1:9" ht="30">
+    <row r="759" spans="1:9">
       <c r="A759" s="28" t="s">
         <v>782</v>
       </c>
@@ -28204,7 +27929,7 @@
       </c>
       <c r="I760" s="30"/>
     </row>
-    <row r="761" spans="1:9" ht="45">
+    <row r="761" spans="1:9" ht="30">
       <c r="A761" s="28" t="s">
         <v>784</v>
       </c>
@@ -28379,7 +28104,7 @@
       </c>
       <c r="I767" s="30"/>
     </row>
-    <row r="768" spans="1:9" ht="30">
+    <row r="768" spans="1:9">
       <c r="A768" s="28" t="s">
         <v>791</v>
       </c>
@@ -28404,7 +28129,7 @@
       </c>
       <c r="I768" s="30"/>
     </row>
-    <row r="769" spans="1:9" ht="30">
+    <row r="769" spans="1:9">
       <c r="A769" s="28" t="s">
         <v>792</v>
       </c>
@@ -28479,7 +28204,7 @@
       </c>
       <c r="I771" s="30"/>
     </row>
-    <row r="772" spans="1:9" ht="45">
+    <row r="772" spans="1:9" ht="30">
       <c r="A772" s="28" t="s">
         <v>795</v>
       </c>
@@ -28529,7 +28254,7 @@
       </c>
       <c r="I773" s="30"/>
     </row>
-    <row r="774" spans="1:9" ht="285">
+    <row r="774" spans="1:9" ht="270">
       <c r="A774" s="28" t="s">
         <v>797</v>
       </c>
@@ -28604,7 +28329,7 @@
       </c>
       <c r="I776" s="33"/>
     </row>
-    <row r="777" spans="1:9" ht="30">
+    <row r="777" spans="1:9">
       <c r="A777" s="28" t="s">
         <v>799</v>
       </c>
@@ -28679,7 +28404,7 @@
       </c>
       <c r="I779" s="30"/>
     </row>
-    <row r="780" spans="1:9" ht="30">
+    <row r="780" spans="1:9">
       <c r="A780" s="28" t="s">
         <v>802</v>
       </c>
@@ -28704,7 +28429,7 @@
       </c>
       <c r="I780" s="30"/>
     </row>
-    <row r="781" spans="1:9" ht="30">
+    <row r="781" spans="1:9">
       <c r="A781" s="28" t="s">
         <v>803</v>
       </c>
@@ -28729,7 +28454,7 @@
       </c>
       <c r="I781" s="30"/>
     </row>
-    <row r="782" spans="1:9" ht="30">
+    <row r="782" spans="1:9">
       <c r="A782" s="28" t="s">
         <v>804</v>
       </c>
@@ -28754,7 +28479,7 @@
       </c>
       <c r="I782" s="30"/>
     </row>
-    <row r="783" spans="1:9" ht="30">
+    <row r="783" spans="1:9">
       <c r="A783" s="28" t="s">
         <v>805</v>
       </c>
@@ -28779,7 +28504,7 @@
       </c>
       <c r="I783" s="30"/>
     </row>
-    <row r="784" spans="1:9" ht="30">
+    <row r="784" spans="1:9">
       <c r="A784" s="28" t="s">
         <v>806</v>
       </c>
@@ -28804,7 +28529,7 @@
       </c>
       <c r="I784" s="30"/>
     </row>
-    <row r="785" spans="1:9" ht="30">
+    <row r="785" spans="1:9">
       <c r="A785" s="28" t="s">
         <v>807</v>
       </c>
@@ -28879,7 +28604,7 @@
       </c>
       <c r="I787" s="30"/>
     </row>
-    <row r="788" spans="1:9" ht="45">
+    <row r="788" spans="1:9" ht="30">
       <c r="A788" s="28" t="s">
         <v>810</v>
       </c>
@@ -28904,7 +28629,7 @@
       </c>
       <c r="I788" s="30"/>
     </row>
-    <row r="789" spans="1:9" ht="30">
+    <row r="789" spans="1:9">
       <c r="A789" s="28" t="s">
         <v>811</v>
       </c>
@@ -28929,7 +28654,7 @@
       </c>
       <c r="I789" s="30"/>
     </row>
-    <row r="790" spans="1:9" ht="30">
+    <row r="790" spans="1:9">
       <c r="A790" s="28" t="s">
         <v>812</v>
       </c>
@@ -28954,7 +28679,7 @@
       </c>
       <c r="I790" s="30"/>
     </row>
-    <row r="791" spans="1:9" ht="30">
+    <row r="791" spans="1:9">
       <c r="A791" s="28" t="s">
         <v>813</v>
       </c>
@@ -29129,7 +28854,7 @@
       </c>
       <c r="I797" s="30"/>
     </row>
-    <row r="798" spans="1:9" ht="30">
+    <row r="798" spans="1:9">
       <c r="A798" s="28" t="s">
         <v>820</v>
       </c>
@@ -29154,7 +28879,7 @@
       </c>
       <c r="I798" s="30"/>
     </row>
-    <row r="799" spans="1:9" ht="30">
+    <row r="799" spans="1:9">
       <c r="A799" s="28" t="s">
         <v>821</v>
       </c>
@@ -29179,7 +28904,7 @@
       </c>
       <c r="I799" s="30"/>
     </row>
-    <row r="800" spans="1:9" ht="30">
+    <row r="800" spans="1:9">
       <c r="A800" s="28" t="s">
         <v>822</v>
       </c>
@@ -29304,7 +29029,7 @@
       </c>
       <c r="I804" s="30"/>
     </row>
-    <row r="805" spans="1:9" ht="30">
+    <row r="805" spans="1:9">
       <c r="A805" s="28" t="s">
         <v>827</v>
       </c>
@@ -29404,7 +29129,7 @@
       </c>
       <c r="I808" s="30"/>
     </row>
-    <row r="809" spans="1:9" ht="30">
+    <row r="809" spans="1:9">
       <c r="A809" s="28" t="s">
         <v>831</v>
       </c>
@@ -29529,7 +29254,7 @@
       </c>
       <c r="I813" s="30"/>
     </row>
-    <row r="814" spans="1:9" ht="30">
+    <row r="814" spans="1:9">
       <c r="A814" s="28" t="s">
         <v>835</v>
       </c>
@@ -29579,7 +29304,7 @@
       </c>
       <c r="I815" s="18"/>
     </row>
-    <row r="816" spans="1:9" ht="30">
+    <row r="816" spans="1:9">
       <c r="A816" s="28" t="s">
         <v>837</v>
       </c>
@@ -29604,7 +29329,7 @@
       </c>
       <c r="I816" s="30"/>
     </row>
-    <row r="817" spans="1:9" ht="45">
+    <row r="817" spans="1:9" ht="30">
       <c r="A817" s="28" t="s">
         <v>838</v>
       </c>
@@ -29752,7 +29477,7 @@
         <v>15</v>
       </c>
       <c r="H822" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I822" s="30"/>
     </row>
@@ -29906,7 +29631,7 @@
       </c>
       <c r="I828" s="30"/>
     </row>
-    <row r="829" spans="1:9" ht="45">
+    <row r="829" spans="1:9" ht="30">
       <c r="A829" s="28" t="s">
         <v>850</v>
       </c>
@@ -30031,7 +29756,7 @@
       </c>
       <c r="I833" s="30"/>
     </row>
-    <row r="834" spans="1:9" ht="45">
+    <row r="834" spans="1:9" ht="30">
       <c r="A834" s="28" t="s">
         <v>855</v>
       </c>
@@ -30056,7 +29781,7 @@
       </c>
       <c r="I834" s="30"/>
     </row>
-    <row r="835" spans="1:9" ht="45">
+    <row r="835" spans="1:9" ht="30">
       <c r="A835" s="28" t="s">
         <v>856</v>
       </c>
@@ -30181,7 +29906,7 @@
       </c>
       <c r="I839" s="30"/>
     </row>
-    <row r="840" spans="1:9" ht="30">
+    <row r="840" spans="1:9">
       <c r="A840" s="28" t="s">
         <v>860</v>
       </c>
@@ -30231,7 +29956,7 @@
       </c>
       <c r="I841" s="30"/>
     </row>
-    <row r="842" spans="1:9" ht="45">
+    <row r="842" spans="1:9" ht="30">
       <c r="A842" s="28" t="s">
         <v>862</v>
       </c>
@@ -30306,7 +30031,7 @@
       </c>
       <c r="I844" s="30"/>
     </row>
-    <row r="845" spans="1:9" ht="45">
+    <row r="845" spans="1:9" ht="30">
       <c r="A845" s="28" t="s">
         <v>865</v>
       </c>
@@ -30356,7 +30081,7 @@
       </c>
       <c r="I846" s="30"/>
     </row>
-    <row r="847" spans="1:9" ht="45">
+    <row r="847" spans="1:9" ht="30">
       <c r="A847" s="28" t="s">
         <v>867</v>
       </c>
@@ -30406,7 +30131,7 @@
       </c>
       <c r="I848" s="30"/>
     </row>
-    <row r="849" spans="1:9" ht="255">
+    <row r="849" spans="1:9" ht="240">
       <c r="A849" s="28" t="s">
         <v>869</v>
       </c>
@@ -30431,7 +30156,7 @@
       </c>
       <c r="I849" s="30"/>
     </row>
-    <row r="850" spans="1:9" ht="45">
+    <row r="850" spans="1:9" ht="30">
       <c r="A850" s="28" t="s">
         <v>870</v>
       </c>
@@ -30456,7 +30181,7 @@
       </c>
       <c r="I850" s="30"/>
     </row>
-    <row r="851" spans="1:9" ht="30">
+    <row r="851" spans="1:9">
       <c r="A851" s="28" t="s">
         <v>871</v>
       </c>
@@ -30531,7 +30256,7 @@
       </c>
       <c r="I853" s="30"/>
     </row>
-    <row r="854" spans="1:9" ht="45">
+    <row r="854" spans="1:9" ht="30">
       <c r="A854" s="28" t="s">
         <v>874</v>
       </c>
@@ -30781,7 +30506,7 @@
       </c>
       <c r="I863" s="30"/>
     </row>
-    <row r="864" spans="1:9" ht="30">
+    <row r="864" spans="1:9">
       <c r="A864" s="28" t="s">
         <v>884</v>
       </c>
@@ -30981,7 +30706,7 @@
       </c>
       <c r="I871" s="30"/>
     </row>
-    <row r="872" spans="1:9" ht="135">
+    <row r="872" spans="1:9" ht="120">
       <c r="A872" s="28" t="s">
         <v>892</v>
       </c>
@@ -31006,7 +30731,7 @@
       </c>
       <c r="I872" s="30"/>
     </row>
-    <row r="873" spans="1:9" ht="30">
+    <row r="873" spans="1:9">
       <c r="A873" s="28" t="s">
         <v>893</v>
       </c>
@@ -31110,7 +30835,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="877" spans="1:9" ht="60">
+    <row r="877" spans="1:9" ht="45">
       <c r="A877" s="28" t="s">
         <v>896</v>
       </c>
@@ -31502,7 +31227,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="891" spans="1:9" ht="45">
+    <row r="891" spans="1:9" ht="30">
       <c r="A891" s="20" t="s">
         <v>910</v>
       </c>
@@ -31529,7 +31254,7 @@
       </c>
       <c r="I891" s="30"/>
     </row>
-    <row r="892" spans="1:9" ht="45">
+    <row r="892" spans="1:9" ht="30">
       <c r="A892" s="20" t="s">
         <v>911</v>
       </c>
@@ -31829,7 +31554,7 @@
       </c>
       <c r="I903" s="30"/>
     </row>
-    <row r="904" spans="1:9" ht="45">
+    <row r="904" spans="1:9" ht="30">
       <c r="A904" s="28" t="s">
         <v>923</v>
       </c>
@@ -31854,11 +31579,11 @@
       </c>
       <c r="I904" s="30"/>
     </row>
-    <row r="905" spans="1:9" ht="75">
+    <row r="905" spans="1:9" ht="60">
       <c r="A905" s="20" t="s">
         <v>2140</v>
       </c>
-      <c r="B905" s="49" t="s">
+      <c r="B905" s="36" t="s">
         <v>2139</v>
       </c>
       <c r="C905" s="33" t="s">
@@ -31879,11 +31604,11 @@
       </c>
       <c r="I905" s="33"/>
     </row>
-    <row r="906" spans="1:9" ht="75">
+    <row r="906" spans="1:9" ht="60">
       <c r="A906" s="20" t="s">
         <v>2141</v>
       </c>
-      <c r="B906" s="49" t="s">
+      <c r="B906" s="36" t="s">
         <v>2139</v>
       </c>
       <c r="C906" s="33" t="s">
@@ -31904,7 +31629,7 @@
       </c>
       <c r="I906" s="33"/>
     </row>
-    <row r="907" spans="1:9" ht="45">
+    <row r="907" spans="1:9" ht="30">
       <c r="A907" s="20" t="s">
         <v>924</v>
       </c>
@@ -32155,7 +31880,7 @@
       </c>
       <c r="I915" s="18"/>
     </row>
-    <row r="916" spans="1:9" ht="45">
+    <row r="916" spans="1:9" ht="30">
       <c r="A916" s="20" t="s">
         <v>933</v>
       </c>
@@ -32211,7 +31936,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="918" spans="1:9" ht="45">
+    <row r="918" spans="1:9" ht="30">
       <c r="A918" s="20" t="s">
         <v>935</v>
       </c>
@@ -32265,7 +31990,7 @@
       </c>
       <c r="I919" s="18"/>
     </row>
-    <row r="920" spans="1:9" ht="45">
+    <row r="920" spans="1:9" ht="30">
       <c r="A920" s="28" t="s">
         <v>937</v>
       </c>
@@ -32319,7 +32044,7 @@
       </c>
       <c r="I921" s="30"/>
     </row>
-    <row r="922" spans="1:9" ht="45">
+    <row r="922" spans="1:9" ht="30">
       <c r="A922" s="28" t="s">
         <v>939</v>
       </c>
@@ -32431,7 +32156,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="926" spans="1:9" ht="45">
+    <row r="926" spans="1:9" ht="30">
       <c r="A926" s="28" t="s">
         <v>943</v>
       </c>
@@ -32487,7 +32212,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="928" spans="1:9" ht="45">
+    <row r="928" spans="1:9" ht="30">
       <c r="A928" s="20" t="s">
         <v>945</v>
       </c>
@@ -32543,7 +32268,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="930" spans="1:9" ht="45">
+    <row r="930" spans="1:9" ht="30">
       <c r="A930" s="28" t="s">
         <v>947</v>
       </c>
@@ -32599,7 +32324,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="932" spans="1:9" ht="45">
+    <row r="932" spans="1:9" ht="30">
       <c r="A932" s="20" t="s">
         <v>949</v>
       </c>
@@ -32655,7 +32380,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="934" spans="1:9" ht="45">
+    <row r="934" spans="1:9" ht="30">
       <c r="A934" s="20" t="s">
         <v>951</v>
       </c>
@@ -32711,7 +32436,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="936" spans="1:9" ht="60">
+    <row r="936" spans="1:9" ht="45">
       <c r="A936" s="32" t="s">
         <v>237</v>
       </c>
@@ -32767,7 +32492,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="938" spans="1:9" ht="75">
+    <row r="938" spans="1:9" ht="60">
       <c r="A938" s="20" t="s">
         <v>239</v>
       </c>
@@ -32825,7 +32550,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="940" spans="1:9" ht="90">
+    <row r="940" spans="1:9" ht="75">
       <c r="A940" s="20" t="s">
         <v>241</v>
       </c>
@@ -32997,7 +32722,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="946" spans="1:9" ht="105">
+    <row r="946" spans="1:9" ht="90">
       <c r="A946" s="32" t="s">
         <v>688</v>
       </c>
@@ -33024,7 +32749,7 @@
       </c>
       <c r="I946" s="33"/>
     </row>
-    <row r="947" spans="1:9" ht="75">
+    <row r="947" spans="1:9" ht="60">
       <c r="A947" s="32" t="s">
         <v>689</v>
       </c>
@@ -33111,7 +32836,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="950" spans="1:9" ht="165">
+    <row r="950" spans="1:9" ht="150">
       <c r="A950" s="32" t="s">
         <v>766</v>
       </c>
@@ -33140,7 +32865,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="951" spans="1:9" ht="165">
+    <row r="951" spans="1:9" ht="150">
       <c r="A951" s="32" t="s">
         <v>767</v>
       </c>
@@ -33169,7 +32894,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="952" spans="1:9" ht="165">
+    <row r="952" spans="1:9" ht="150">
       <c r="A952" s="32" t="s">
         <v>768</v>
       </c>
@@ -33227,7 +32952,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="954" spans="1:9" ht="165">
+    <row r="954" spans="1:9" ht="150">
       <c r="A954" s="32" t="s">
         <v>770</v>
       </c>
@@ -33258,6 +32983,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -33265,92 +32995,87 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A687:B687 E937:E940 D687:I687 A876:H876 A941:I954 A20:I686 I667:I876 A688:I875 A877:I936">
-    <cfRule type="expression" dxfId="45" priority="85">
+    <cfRule type="expression" dxfId="40" priority="85">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="86">
+    <cfRule type="expression" dxfId="39" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="93">
+    <cfRule type="expression" dxfId="38" priority="93">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A687:B687 E937:E940 D687:I687 A876:H876 A941:I954 A20:I686 I667:I876 A688:I875 A877:I936">
-    <cfRule type="expression" dxfId="42" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="40">
+    <cfRule type="expression" dxfId="36" priority="40">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F941:F954 F20:F936">
-    <cfRule type="expression" dxfId="39" priority="45">
+    <cfRule type="expression" dxfId="34" priority="45">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="46">
+    <cfRule type="expression" dxfId="33" priority="46">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C687">
-    <cfRule type="expression" dxfId="37" priority="24">
+    <cfRule type="expression" dxfId="32" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="25">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="26">
+    <cfRule type="expression" dxfId="30" priority="26">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C687">
-    <cfRule type="expression" dxfId="34" priority="21">
+    <cfRule type="expression" dxfId="29" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="22">
+    <cfRule type="expression" dxfId="28" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="23">
+    <cfRule type="expression" dxfId="27" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A937:D940 F937:I940">
-    <cfRule type="expression" dxfId="31" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="19">
+    <cfRule type="expression" dxfId="25" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="20">
+    <cfRule type="expression" dxfId="24" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A937:D940 F937:I940">
-    <cfRule type="expression" dxfId="28" priority="13">
+    <cfRule type="expression" dxfId="23" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="14">
+    <cfRule type="expression" dxfId="22" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="15">
+    <cfRule type="expression" dxfId="21" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F937:F940">
-    <cfRule type="expression" dxfId="25" priority="16">
+    <cfRule type="expression" dxfId="20" priority="16">
       <formula>NOT(VLOOKUP(F937,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="17">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>(VLOOKUP(F937,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33388,12 +33113,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33446,15 +33168,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33475,15 +33206,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update capture code in test suite and add SharePoint 2019 ptfconfig file.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SharePoint-TestSuite\Docs\MS-WEBSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCA9A84-1605-4713-83D7-AA9A0B2D2266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFBAD54-8A85-45AC-B848-2C9459CEEB46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6693" uniqueCount="2158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6697" uniqueCount="2159">
   <si>
     <t>Req ID</t>
   </si>
@@ -7620,14 +7620,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does not support this method[IsSPO]. (&lt;3&gt; Section 2.2.4.2: This attribute[FarmId] is not returned in Windows SharePoint Services 2.0, Windows SharePoint Services 3.0 and SharePoint Foundation 2010.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix B: Product Behavior] Implementation does not support this method[SiteId]. (&lt;3&gt; Section 2.2.4.2: This attribute[FarmId] is not returned in Windows SharePoint Services 2.0, Windows SharePoint Services 3.0 , SharePoint Foundation 2010 and SharePoint Foundation 2013.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior]Implementation does support this method [IsSPO]. (&lt;3&gt; Section 2.2.4.2: This attribute is returned in Microsoft SharePoint Server 2016 and above follow this behavior.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7816,6 +7808,18 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Implementation does support this[UpdateContentTypeXmlDocument] operation.(&lt;25&gt;Windows SharePoint Services 3.0 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does not support this method[SiteId]. (&lt;3&gt; Section 2.2.4.2:  This attribute is not returned in Windows SharePoint Services 2.0, Windows SharePoint Services 3.0 and SharePoint Foundation 2010.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does not support this method[IsSPO]. (&lt;4&gt; Section 2.2.4.2:  This attribute is not returned in Windows SharePoint Services 2.0, Windows SharePoint Services 3.0, SharePoint Foundation 2010 and SharePoint Foundation 2013.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7877,6 +7881,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -8105,6 +8110,24 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8129,147 +8152,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8608,6 +8495,124 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8737,34 +8742,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I959" tableType="xml" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I959" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I959" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="37">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="36">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="35">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="33">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="32">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="31">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="30">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8773,12 +8778,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9150,7 +9155,7 @@
       <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="36" t="s">
         <v>2066</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -9162,127 +9167,127 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -9295,12 +9300,12 @@
       <c r="C12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -9313,12 +9318,12 @@
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -9331,12 +9336,12 @@
       <c r="C14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -9349,60 +9354,60 @@
       <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="48" t="s">
         <v>1889</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="4"/>
       <c r="L18" s="3"/>
     </row>
@@ -31120,14 +31125,16 @@
     </row>
     <row r="882" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A882" s="20" t="s">
-        <v>2114</v>
-      </c>
-      <c r="B882" s="22"/>
+        <v>2112</v>
+      </c>
+      <c r="B882" s="22" t="s">
+        <v>2158</v>
+      </c>
       <c r="C882" s="18" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D882" s="20" t="s">
         <v>2109</v>
-      </c>
-      <c r="D882" s="20" t="s">
-        <v>2111</v>
       </c>
       <c r="E882" s="27" t="s">
         <v>22</v>
@@ -31145,14 +31152,16 @@
     </row>
     <row r="883" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A883" s="20" t="s">
-        <v>2113</v>
-      </c>
-      <c r="B883" s="22"/>
+        <v>2111</v>
+      </c>
+      <c r="B883" s="22" t="s">
+        <v>2158</v>
+      </c>
       <c r="C883" s="18" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
       <c r="D883" s="20" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="E883" s="27" t="s">
         <v>22</v>
@@ -31172,14 +31181,16 @@
     </row>
     <row r="884" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A884" s="20" t="s">
-        <v>2115</v>
-      </c>
-      <c r="B884" s="22"/>
+        <v>2113</v>
+      </c>
+      <c r="B884" s="22" t="s">
+        <v>2158</v>
+      </c>
       <c r="C884" s="18" t="s">
-        <v>2108</v>
+        <v>2157</v>
       </c>
       <c r="D884" s="20" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="E884" s="27" t="s">
         <v>22</v>
@@ -31197,14 +31208,16 @@
     </row>
     <row r="885" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A885" s="20" t="s">
-        <v>2116</v>
-      </c>
-      <c r="B885" s="22"/>
+        <v>2114</v>
+      </c>
+      <c r="B885" s="22" t="s">
+        <v>2158</v>
+      </c>
       <c r="C885" s="18" t="s">
-        <v>2107</v>
+        <v>2108</v>
       </c>
       <c r="D885" s="20" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="E885" s="27" t="s">
         <v>22</v>
@@ -31230,7 +31243,7 @@
         <v>7</v>
       </c>
       <c r="C886" s="18" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="D886" s="20" t="s">
         <v>1863</v>
@@ -31257,7 +31270,7 @@
         <v>7</v>
       </c>
       <c r="C887" s="18" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="D887" s="20" t="s">
         <v>1863</v>
@@ -31286,7 +31299,7 @@
         <v>7</v>
       </c>
       <c r="C888" s="18" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="D888" s="20" t="s">
         <v>1864</v>
@@ -31313,7 +31326,7 @@
         <v>7</v>
       </c>
       <c r="C889" s="18" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="D889" s="20" t="s">
         <v>1864</v>
@@ -31342,7 +31355,7 @@
         <v>7</v>
       </c>
       <c r="C890" s="18" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="D890" s="20" t="s">
         <v>1865</v>
@@ -31369,7 +31382,7 @@
         <v>7</v>
       </c>
       <c r="C891" s="18" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="D891" s="20" t="s">
         <v>1865</v>
@@ -31398,7 +31411,7 @@
         <v>7</v>
       </c>
       <c r="C892" s="18" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="D892" s="20" t="s">
         <v>1866</v>
@@ -31425,7 +31438,7 @@
         <v>7</v>
       </c>
       <c r="C893" s="18" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="D893" s="20" t="s">
         <v>1866</v>
@@ -31454,7 +31467,7 @@
         <v>7</v>
       </c>
       <c r="C894" s="18" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="D894" s="20" t="s">
         <v>1859</v>
@@ -31481,7 +31494,7 @@
         <v>7</v>
       </c>
       <c r="C895" s="18" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="D895" s="20" t="s">
         <v>1859</v>
@@ -31510,7 +31523,7 @@
         <v>7</v>
       </c>
       <c r="C896" s="18" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="D896" s="20" t="s">
         <v>1860</v>
@@ -31537,7 +31550,7 @@
         <v>7</v>
       </c>
       <c r="C897" s="18" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="D897" s="27"/>
       <c r="E897" s="27" t="s">
@@ -31912,7 +31925,7 @@
         <v>7</v>
       </c>
       <c r="C912" s="18" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="D912" s="20" t="s">
         <v>1867</v>
@@ -31939,7 +31952,7 @@
         <v>7</v>
       </c>
       <c r="C913" s="18" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
       <c r="D913" s="20" t="s">
         <v>1867</v>
@@ -31968,7 +31981,7 @@
         <v>7</v>
       </c>
       <c r="C914" s="18" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
       <c r="D914" s="20" t="s">
         <v>1868</v>
@@ -31995,7 +32008,7 @@
         <v>7</v>
       </c>
       <c r="C915" s="18" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
       <c r="D915" s="20" t="s">
         <v>1869</v>
@@ -32022,7 +32035,7 @@
         <v>7</v>
       </c>
       <c r="C916" s="18" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
       <c r="D916" s="27" t="s">
         <v>1869</v>
@@ -32051,7 +32064,7 @@
         <v>7</v>
       </c>
       <c r="C917" s="18" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="D917" s="27" t="s">
         <v>1868</v>
@@ -32080,7 +32093,7 @@
         <v>7</v>
       </c>
       <c r="C918" s="18" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
       <c r="D918" s="27" t="s">
         <v>1870</v>
@@ -32107,7 +32120,7 @@
         <v>7</v>
       </c>
       <c r="C919" s="18" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="D919" s="27" t="s">
         <v>1870</v>
@@ -32136,7 +32149,7 @@
         <v>7</v>
       </c>
       <c r="C920" s="18" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="D920" s="27" t="s">
         <v>1860</v>
@@ -32163,7 +32176,7 @@
         <v>7</v>
       </c>
       <c r="C921" s="18" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="D921" s="27" t="s">
         <v>1871</v>
@@ -32190,7 +32203,7 @@
         <v>7</v>
       </c>
       <c r="C922" s="18" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
       <c r="D922" s="27" t="s">
         <v>1871</v>
@@ -32219,7 +32232,7 @@
         <v>7</v>
       </c>
       <c r="C923" s="18" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="D923" s="27" t="s">
         <v>1872</v>
@@ -32246,7 +32259,7 @@
         <v>7</v>
       </c>
       <c r="C924" s="18" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="D924" s="27" t="s">
         <v>1872</v>
@@ -32273,7 +32286,7 @@
         <v>7</v>
       </c>
       <c r="C925" s="18" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="D925" s="27" t="s">
         <v>1873</v>
@@ -32300,7 +32313,7 @@
         <v>7</v>
       </c>
       <c r="C926" s="18" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="D926" s="27" t="s">
         <v>1873</v>
@@ -32327,7 +32340,7 @@
         <v>7</v>
       </c>
       <c r="C927" s="18" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
       <c r="D927" s="27" t="s">
         <v>1874</v>
@@ -32354,7 +32367,7 @@
         <v>7</v>
       </c>
       <c r="C928" s="18" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
       <c r="D928" s="27" t="s">
         <v>1874</v>
@@ -32383,7 +32396,7 @@
         <v>7</v>
       </c>
       <c r="C929" s="18" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="D929" s="27" t="s">
         <v>1875</v>
@@ -32410,7 +32423,7 @@
         <v>7</v>
       </c>
       <c r="C930" s="18" t="s">
-        <v>2147</v>
+        <v>2145</v>
       </c>
       <c r="D930" s="27" t="s">
         <v>1875</v>
@@ -32439,7 +32452,7 @@
         <v>7</v>
       </c>
       <c r="C931" s="18" t="s">
-        <v>2148</v>
+        <v>2146</v>
       </c>
       <c r="D931" s="27" t="s">
         <v>1876</v>
@@ -32466,7 +32479,7 @@
         <v>7</v>
       </c>
       <c r="C932" s="18" t="s">
-        <v>2149</v>
+        <v>2147</v>
       </c>
       <c r="D932" s="27" t="s">
         <v>1876</v>
@@ -32495,7 +32508,7 @@
         <v>7</v>
       </c>
       <c r="C933" s="18" t="s">
-        <v>2150</v>
+        <v>2148</v>
       </c>
       <c r="D933" s="27" t="s">
         <v>1877</v>
@@ -32522,7 +32535,7 @@
         <v>7</v>
       </c>
       <c r="C934" s="18" t="s">
-        <v>2151</v>
+        <v>2149</v>
       </c>
       <c r="D934" s="27" t="s">
         <v>1877</v>
@@ -32551,7 +32564,7 @@
         <v>7</v>
       </c>
       <c r="C935" s="18" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="D935" s="27" t="s">
         <v>1878</v>
@@ -32578,7 +32591,7 @@
         <v>7</v>
       </c>
       <c r="C936" s="18" t="s">
-        <v>2153</v>
+        <v>2151</v>
       </c>
       <c r="D936" s="27" t="s">
         <v>1878</v>
@@ -32607,7 +32620,7 @@
         <v>7</v>
       </c>
       <c r="C937" s="18" t="s">
-        <v>2154</v>
+        <v>2152</v>
       </c>
       <c r="D937" s="27" t="s">
         <v>1879</v>
@@ -32634,7 +32647,7 @@
         <v>7</v>
       </c>
       <c r="C938" s="18" t="s">
-        <v>2155</v>
+        <v>2153</v>
       </c>
       <c r="D938" s="27" t="s">
         <v>1879</v>
@@ -32663,7 +32676,7 @@
         <v>7</v>
       </c>
       <c r="C939" s="18" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="D939" s="27" t="s">
         <v>1880</v>
@@ -32690,7 +32703,7 @@
         <v>7</v>
       </c>
       <c r="C940" s="18" t="s">
-        <v>2157</v>
+        <v>2155</v>
       </c>
       <c r="D940" s="27" t="s">
         <v>1880</v>
@@ -33258,11 +33271,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -33270,87 +33278,92 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A689:B689 E942:E945 D689:I689 A877:H877 A946:I959 I669:I877 A690:I876 A20:I688 A878:I941">
-    <cfRule type="expression" dxfId="21" priority="85">
+    <cfRule type="expression" dxfId="40" priority="85">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="86">
+    <cfRule type="expression" dxfId="39" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="93">
+    <cfRule type="expression" dxfId="38" priority="93">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A689:B689 E942:E945 D689:I689 A877:H877 A946:I959 I669:I877 A690:I876 A20:I688 A878:I941">
-    <cfRule type="expression" dxfId="18" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="40">
+    <cfRule type="expression" dxfId="36" priority="40">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="41">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F946:F959 F20:F941">
-    <cfRule type="expression" dxfId="15" priority="45">
+    <cfRule type="expression" dxfId="34" priority="45">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="46">
+    <cfRule type="expression" dxfId="33" priority="46">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C689">
-    <cfRule type="expression" dxfId="13" priority="24">
+    <cfRule type="expression" dxfId="32" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="25">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="26">
+    <cfRule type="expression" dxfId="30" priority="26">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C689">
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="29" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="28" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="23">
+    <cfRule type="expression" dxfId="27" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A942:D945 F942:I945">
-    <cfRule type="expression" dxfId="7" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="19">
+    <cfRule type="expression" dxfId="25" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="20">
+    <cfRule type="expression" dxfId="24" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A942:D945 F942:I945">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="23" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="14">
+    <cfRule type="expression" dxfId="22" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="15">
+    <cfRule type="expression" dxfId="21" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F942:F945">
-    <cfRule type="expression" dxfId="1" priority="16">
+    <cfRule type="expression" dxfId="20" priority="16">
       <formula>NOT(VLOOKUP(F942,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="17">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>(VLOOKUP(F942,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33388,12 +33401,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -33442,6 +33449,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -33452,20 +33465,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33480,6 +33479,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated some schema and remove preview.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WEBSS/MS-WEBSS_RequirementSpecification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Interop-TestSuites\SharePoint\Docs\MS-WEBSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Interop\TestSuite1\SharePoint\Docs\MS-WEBSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C36393-E3DB-437E-BE0F-C2DA601D0C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994E913C-011B-40E0-83A7-2CA654B2ACEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6650,25 +6650,6 @@
     <t>[In Message Processing Events and Sequencing Rules] [WSDL operation description]  RemoveContentTypeXmlDocument: Removes an XML document in the XML document collection of a site content type.</t>
   </si>
   <si>
-    <t>[In CreateContentType]  This element [CreateContentType] is defined as follows:
- &lt;s:element name="CreateContentType"&gt;
-  &lt;s:complexType&gt;
-    &lt;s:sequence&gt;
-      &lt;s:element name="displayName" type="s:string" minOccurs="1"/&gt;
-      &lt;s:element name="parentType" type="s:string" minOccurs="1"/&gt;
-      &lt;s:element name="newFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
-      &lt;s:element name="contentTypeProperties" minOccurs="1"&gt;
-        &lt;s:complexType&gt;
-          &lt;s:sequence&gt;
-            &lt;s:element name="ContentType" type="ContentTypePropertyDefinition" minOccurs="0" /&gt;
-          &lt;/s:sequence&gt;
-        &lt;/s:complexType&gt;
-      &lt;/s:element&gt;
-    &lt;/s:sequence&gt;
-  &lt;/s:complexType&gt;
-&lt;/s:element&gt;</t>
-  </si>
-  <si>
     <t>[In CreateContentType] parentType: It MUST conform to the ContentTypeId type, as specified in [MS-WSSCAML] section 2.3.1.4.</t>
   </si>
   <si>
@@ -7205,26 +7186,6 @@
     <t>MS-WEBSS_R822001</t>
   </si>
   <si>
-    <t>[In UpdateContentType] This element[UpdateContentType] is defined as follows:
-&lt;s:element name="UpdateContentType"&gt;
-  &lt;s:complexType&gt;
-    &lt;s:sequence&gt;
-      &lt;s:element name="contentTypeId" type="s:string" minOccurs="0"/&gt;
-      &lt;s:element name="contentTypeProperties" minOccurs="1"&gt;
-        &lt;s:complexType&gt;
-          &lt;s:sequence&gt;
-            &lt;s:element name="ContentType" type="ContentTypePropertyDefinition" minOccurs="0" /&gt;
-          &lt;/s:sequence&gt;
-        &lt;/s:complexType&gt;
-      &lt;/s:element&gt;
-      &lt;s:element name="newFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
-      &lt;s:element name="updateFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
-      &lt;s:element name="deleteFields" type="DeleteFieldsDefinition" minOccurs="0"/&gt;
-    &lt;/s:sequence&gt;
-  &lt;/s:complexType&gt;
-&lt;/s:element&gt;</t>
-  </si>
-  <si>
     <t>[In UpdateContentType] contentTypeId: It MUST conform to the ContentTypeId type, as specified in [MS-WSSCAML] section 2.3.1.4.</t>
   </si>
   <si>
@@ -7357,10 +7318,6 @@
     <t>[In UpdateColumns] Method: If the Method element does not contain an ID attribute, the server [does not add, update, or delete columns and]does not return an ErrorCode.</t>
   </si>
   <si>
-    <t>10.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In Transport] Protocol messages MUST be formatted as specified in [SOAP1.2-1/2007] section 5, SOAP Message Construct.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7826,6 +7783,48 @@
   <si>
     <t>[In Messages] [Message] GetAllSubWebCollectionSoapOut
  [Description] The response to a request for the title and URL of all sites in the site collection.</t>
+  </si>
+  <si>
+    <t>[In CreateContentType]  This element [CreateContentType] is defined as follows:
+ &lt;s:element name="CreateContentType"&gt;
+  &lt;s:complexType&gt;
+    &lt;s:sequence&gt;
+      &lt;s:element name="displayName" type="s:string" minOccurs="1"/&gt;
+      &lt;s:element name="parentType" type="s:string" minOccurs="1"/&gt;
+      &lt;s:element name="newFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
+      &lt;s:element name="contentTypeProperties" minOccurs="0" maxOccurs="1"&gt;
+        &lt;s:complexType&gt;
+          &lt;s:sequence&gt;
+            &lt;s:element name="ContentType" type="ContentTypePropertyDefinition" minOccurs="0" /&gt;
+          &lt;/s:sequence&gt;
+        &lt;/s:complexType&gt;
+      &lt;/s:element&gt;
+    &lt;/s:sequence&gt;
+  &lt;/s:complexType&gt;
+&lt;/s:element&gt;</t>
+  </si>
+  <si>
+    <t>[In UpdateContentType] This element[UpdateContentType] is defined as follows:
+&lt;s:element name="UpdateContentType"&gt;
+  &lt;s:complexType&gt;
+    &lt;s:sequence&gt;
+      &lt;s:element name="contentTypeId" type="s:string" minOccurs="0"/&gt;
+      &lt;s:element name="contentTypeProperties" minOccurs="0" maxOccurs="1"&gt;
+        &lt;s:complexType&gt;
+          &lt;s:sequence&gt;
+            &lt;s:element name="ContentType" type="ContentTypePropertyDefinition" minOccurs="0" /&gt;
+          &lt;/s:sequence&gt;
+        &lt;/s:complexType&gt;
+      &lt;/s:element&gt;
+      &lt;s:element name="newFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
+      &lt;s:element name="updateFields" type="AddOrUpdateFieldsDefinition" minOccurs="0"/&gt;
+      &lt;s:element name="deleteFields" type="DeleteFieldsDefinition" minOccurs="0"/&gt;
+    &lt;/s:sequence&gt;
+  &lt;/s:complexType&gt;
+&lt;/s:element&gt;</t>
+  </si>
+  <si>
+    <t>14.1</t>
   </si>
 </sst>
 </file>
@@ -8118,21 +8117,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8156,6 +8140,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9118,8 +9117,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L273" sqref="L273"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9163,138 +9162,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>2044</v>
+        <v>2159</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>1909</v>
       </c>
       <c r="F3" s="10">
-        <v>43634</v>
+        <v>44474</v>
       </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -9307,12 +9306,12 @@
       <c r="C12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10">
@@ -9325,12 +9324,12 @@
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">
@@ -9343,12 +9342,12 @@
       <c r="C14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10">
@@ -9361,60 +9360,60 @@
       <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="30">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>1867</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="30">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="4"/>
       <c r="L18" s="3"/>
     </row>
@@ -9533,7 +9532,7 @@
         <v>2.1</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20" t="s">
@@ -9583,7 +9582,7 @@
         <v>2.1</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>2046</v>
+        <v>2043</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20" t="s">
@@ -9633,7 +9632,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>2047</v>
+        <v>2044</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20" t="s">
@@ -9783,7 +9782,7 @@
         <v>950</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="27" t="s">
@@ -10210,7 +10209,7 @@
         <v>954</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>2049</v>
+        <v>2046</v>
       </c>
       <c r="D50" s="27"/>
       <c r="E50" s="27" t="s">
@@ -10354,10 +10353,10 @@
     </row>
     <row r="56" spans="1:9" ht="45">
       <c r="A56" s="20" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
       <c r="C56" s="29" t="s">
         <v>1132</v>
@@ -10381,13 +10380,13 @@
     </row>
     <row r="57" spans="1:9" ht="45">
       <c r="A57" s="20" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="27" t="s">
@@ -10403,18 +10402,18 @@
         <v>17</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="45">
       <c r="A58" s="20" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>2052</v>
+        <v>2049</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="27" t="s">
@@ -10430,18 +10429,18 @@
         <v>17</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="45">
       <c r="A59" s="20" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="B59" s="28" t="s">
         <v>954</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>2053</v>
+        <v>2050</v>
       </c>
       <c r="D59" s="27"/>
       <c r="E59" s="27" t="s">
@@ -10468,7 +10467,7 @@
         <v>954</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="D60" s="27"/>
       <c r="E60" s="27" t="s">
@@ -10495,7 +10494,7 @@
         <v>954</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>2055</v>
+        <v>2052</v>
       </c>
       <c r="D61" s="27"/>
       <c r="E61" s="27" t="s">
@@ -10522,7 +10521,7 @@
         <v>954</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="D62" s="27"/>
       <c r="E62" s="27" t="s">
@@ -11024,7 +11023,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="27" t="s">
@@ -11174,7 +11173,7 @@
         <v>962</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>2139</v>
+        <v>2136</v>
       </c>
       <c r="D88" s="27"/>
       <c r="E88" s="27" t="s">
@@ -12324,7 +12323,7 @@
         <v>33</v>
       </c>
       <c r="C134" s="18" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
       <c r="D134" s="27"/>
       <c r="E134" s="27" t="s">
@@ -12926,7 +12925,7 @@
         <v>967</v>
       </c>
       <c r="C158" s="18" t="s">
-        <v>1923</v>
+        <v>2157</v>
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27" t="s">
@@ -13579,13 +13578,13 @@
     </row>
     <row r="183" spans="1:9" ht="30">
       <c r="A183" s="20" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B183" s="22" t="s">
         <v>967</v>
       </c>
       <c r="C183" s="32" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="D183" s="31"/>
       <c r="E183" s="27" t="s">
@@ -13760,7 +13759,7 @@
         <v>968</v>
       </c>
       <c r="C190" s="18" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="D190" s="27"/>
       <c r="E190" s="27" t="s">
@@ -13804,13 +13803,13 @@
     </row>
     <row r="192" spans="1:9" ht="30">
       <c r="A192" s="20" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B192" s="28" t="s">
         <v>968</v>
       </c>
       <c r="C192" s="32" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="D192" s="31"/>
       <c r="E192" s="31" t="s">
@@ -13835,7 +13834,7 @@
         <v>34</v>
       </c>
       <c r="C193" s="18" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="D193" s="27"/>
       <c r="E193" s="27" t="s">
@@ -14210,7 +14209,7 @@
         <v>973</v>
       </c>
       <c r="C208" s="18" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="D208" s="27"/>
       <c r="E208" s="27" t="s">
@@ -14260,7 +14259,7 @@
         <v>973</v>
       </c>
       <c r="C210" s="18" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="D210" s="27"/>
       <c r="E210" s="27" t="s">
@@ -14437,7 +14436,7 @@
         <v>975</v>
       </c>
       <c r="C217" s="18" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="D217" s="27"/>
       <c r="E217" s="27" t="s">
@@ -14589,7 +14588,7 @@
         <v>975</v>
       </c>
       <c r="C223" s="18" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
       <c r="D223" s="27"/>
       <c r="E223" s="27" t="s">
@@ -14639,7 +14638,7 @@
         <v>976</v>
       </c>
       <c r="C225" s="18" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="D225" s="27"/>
       <c r="E225" s="27" t="s">
@@ -14664,7 +14663,7 @@
         <v>976</v>
       </c>
       <c r="C226" s="18" t="s">
-        <v>2141</v>
+        <v>2138</v>
       </c>
       <c r="D226" s="27"/>
       <c r="E226" s="27" t="s">
@@ -14789,7 +14788,7 @@
         <v>979</v>
       </c>
       <c r="C231" s="18" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="D231" s="27"/>
       <c r="E231" s="27" t="s">
@@ -14814,7 +14813,7 @@
         <v>979</v>
       </c>
       <c r="C232" s="18" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="D232" s="27"/>
       <c r="E232" s="27" t="s">
@@ -14839,7 +14838,7 @@
         <v>980</v>
       </c>
       <c r="C233" s="18" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="D233" s="27"/>
       <c r="E233" s="27" t="s">
@@ -14864,7 +14863,7 @@
         <v>980</v>
       </c>
       <c r="C234" s="18" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="D234" s="27"/>
       <c r="E234" s="27" t="s">
@@ -14889,7 +14888,7 @@
         <v>980</v>
       </c>
       <c r="C235" s="18" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="D235" s="27"/>
       <c r="E235" s="27" t="s">
@@ -14908,13 +14907,13 @@
     </row>
     <row r="236" spans="1:9" ht="30">
       <c r="A236" s="20" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B236" s="28" t="s">
         <v>980</v>
       </c>
       <c r="C236" s="32" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="D236" s="31"/>
       <c r="E236" s="31" t="s">
@@ -14939,7 +14938,7 @@
         <v>981</v>
       </c>
       <c r="C237" s="18" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="D237" s="27"/>
       <c r="E237" s="27" t="s">
@@ -14964,7 +14963,7 @@
         <v>981</v>
       </c>
       <c r="C238" s="18" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="D238" s="27"/>
       <c r="E238" s="27" t="s">
@@ -15039,7 +15038,7 @@
         <v>982</v>
       </c>
       <c r="C241" s="18" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="D241" s="27"/>
       <c r="E241" s="27" t="s">
@@ -15141,7 +15140,7 @@
         <v>982</v>
       </c>
       <c r="C245" s="18" t="s">
-        <v>2143</v>
+        <v>2140</v>
       </c>
       <c r="D245" s="27"/>
       <c r="E245" s="27" t="s">
@@ -15216,7 +15215,7 @@
         <v>982</v>
       </c>
       <c r="C248" s="18" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="D248" s="27"/>
       <c r="E248" s="27" t="s">
@@ -15266,7 +15265,7 @@
         <v>983</v>
       </c>
       <c r="C250" s="18" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="D250" s="27"/>
       <c r="E250" s="27" t="s">
@@ -15291,7 +15290,7 @@
         <v>983</v>
       </c>
       <c r="C251" s="18" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="D251" s="27"/>
       <c r="E251" s="27" t="s">
@@ -15316,7 +15315,7 @@
         <v>984</v>
       </c>
       <c r="C252" s="18" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="D252" s="27"/>
       <c r="E252" s="27" t="s">
@@ -15391,7 +15390,7 @@
         <v>985</v>
       </c>
       <c r="C255" s="18" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="D255" s="27"/>
       <c r="E255" s="27" t="s">
@@ -15416,7 +15415,7 @@
         <v>985</v>
       </c>
       <c r="C256" s="18" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="D256" s="27"/>
       <c r="E256" s="27" t="s">
@@ -15491,7 +15490,7 @@
         <v>986</v>
       </c>
       <c r="C259" s="18" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="D259" s="27"/>
       <c r="E259" s="27" t="s">
@@ -15516,7 +15515,7 @@
         <v>986</v>
       </c>
       <c r="C260" s="18" t="s">
-        <v>2147</v>
+        <v>2144</v>
       </c>
       <c r="D260" s="27"/>
       <c r="E260" s="27" t="s">
@@ -15566,7 +15565,7 @@
         <v>988</v>
       </c>
       <c r="C262" s="18" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="D262" s="27"/>
       <c r="E262" s="27" t="s">
@@ -15616,7 +15615,7 @@
         <v>988</v>
       </c>
       <c r="C264" s="18" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D264" s="27"/>
       <c r="E264" s="27" t="s">
@@ -15635,7 +15634,7 @@
     </row>
     <row r="265" spans="1:9" ht="45">
       <c r="A265" s="20" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
       <c r="B265" s="28" t="s">
         <v>988</v>
@@ -15654,7 +15653,7 @@
         <v>15</v>
       </c>
       <c r="H265" s="20" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
       <c r="I265" s="18"/>
     </row>
@@ -15666,7 +15665,7 @@
         <v>989</v>
       </c>
       <c r="C266" s="18" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="D266" s="27"/>
       <c r="E266" s="27" t="s">
@@ -15841,7 +15840,7 @@
         <v>990</v>
       </c>
       <c r="C273" s="18" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="D273" s="27"/>
       <c r="E273" s="27" t="s">
@@ -15866,7 +15865,7 @@
         <v>990</v>
       </c>
       <c r="C274" s="18" t="s">
-        <v>2159</v>
+        <v>2156</v>
       </c>
       <c r="D274" s="27"/>
       <c r="E274" s="27" t="s">
@@ -15966,7 +15965,7 @@
         <v>992</v>
       </c>
       <c r="C278" s="18" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="D278" s="27"/>
       <c r="E278" s="27" t="s">
@@ -16041,7 +16040,7 @@
         <v>993</v>
       </c>
       <c r="C281" s="18" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="D281" s="27"/>
       <c r="E281" s="27" t="s">
@@ -16066,7 +16065,7 @@
         <v>993</v>
       </c>
       <c r="C282" s="18" t="s">
-        <v>2148</v>
+        <v>2145</v>
       </c>
       <c r="D282" s="27"/>
       <c r="E282" s="27" t="s">
@@ -16116,7 +16115,7 @@
         <v>995</v>
       </c>
       <c r="C284" s="18" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="D284" s="27"/>
       <c r="E284" s="27" t="s">
@@ -16216,7 +16215,7 @@
         <v>995</v>
       </c>
       <c r="C288" s="18" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="D288" s="27"/>
       <c r="E288" s="27" t="s">
@@ -16341,7 +16340,7 @@
         <v>996</v>
       </c>
       <c r="C293" s="18" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="D293" s="27"/>
       <c r="E293" s="27" t="s">
@@ -16841,7 +16840,7 @@
         <v>1002</v>
       </c>
       <c r="C313" s="18" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="D313" s="27"/>
       <c r="E313" s="27" t="s">
@@ -16991,7 +16990,7 @@
         <v>1003</v>
       </c>
       <c r="C319" s="18" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="D319" s="27"/>
       <c r="E319" s="27" t="s">
@@ -17116,7 +17115,7 @@
         <v>1003</v>
       </c>
       <c r="C324" s="18" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D324" s="27"/>
       <c r="E324" s="27" t="s">
@@ -17416,7 +17415,7 @@
         <v>1008</v>
       </c>
       <c r="C336" s="18" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="D336" s="27"/>
       <c r="E336" s="27" t="s">
@@ -17485,13 +17484,13 @@
     </row>
     <row r="339" spans="1:9" ht="30">
       <c r="A339" s="20" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B339" s="28" t="s">
         <v>1008</v>
       </c>
       <c r="C339" s="32" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="D339" s="31"/>
       <c r="E339" s="31" t="s">
@@ -17666,7 +17665,7 @@
         <v>1009</v>
       </c>
       <c r="C346" s="18" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D346" s="27"/>
       <c r="E346" s="27" t="s">
@@ -17716,7 +17715,7 @@
         <v>1009</v>
       </c>
       <c r="C348" s="18" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D348" s="27"/>
       <c r="E348" s="27" t="s">
@@ -17791,7 +17790,7 @@
         <v>1009</v>
       </c>
       <c r="C351" s="18" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="D351" s="27"/>
       <c r="E351" s="27" t="s">
@@ -17816,7 +17815,7 @@
         <v>1009</v>
       </c>
       <c r="C352" s="18" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D352" s="27"/>
       <c r="E352" s="27" t="s">
@@ -18366,7 +18365,7 @@
         <v>1010</v>
       </c>
       <c r="C374" s="18" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="D374" s="27"/>
       <c r="E374" s="27" t="s">
@@ -18391,7 +18390,7 @@
         <v>1010</v>
       </c>
       <c r="C375" s="18" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
       <c r="D375" s="27"/>
       <c r="E375" s="27" t="s">
@@ -18493,7 +18492,7 @@
         <v>1011</v>
       </c>
       <c r="C379" s="18" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="D379" s="27"/>
       <c r="E379" s="27" t="s">
@@ -18518,7 +18517,7 @@
         <v>1011</v>
       </c>
       <c r="C380" s="18" t="s">
-        <v>2149</v>
+        <v>2146</v>
       </c>
       <c r="D380" s="27"/>
       <c r="E380" s="27" t="s">
@@ -18543,7 +18542,7 @@
         <v>1012</v>
       </c>
       <c r="C381" s="18" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="D381" s="27"/>
       <c r="E381" s="27" t="s">
@@ -18618,7 +18617,7 @@
         <v>1013</v>
       </c>
       <c r="C384" s="18" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="D384" s="27"/>
       <c r="E384" s="27" t="s">
@@ -18693,7 +18692,7 @@
         <v>1014</v>
       </c>
       <c r="C387" s="18" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D387" s="27"/>
       <c r="E387" s="27" t="s">
@@ -18718,7 +18717,7 @@
         <v>1014</v>
       </c>
       <c r="C388" s="18" t="s">
-        <v>2150</v>
+        <v>2147</v>
       </c>
       <c r="D388" s="27"/>
       <c r="E388" s="27" t="s">
@@ -18743,7 +18742,7 @@
         <v>1015</v>
       </c>
       <c r="C389" s="18" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="D389" s="27"/>
       <c r="E389" s="27" t="s">
@@ -18793,7 +18792,7 @@
         <v>1016</v>
       </c>
       <c r="C391" s="18" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="D391" s="27"/>
       <c r="E391" s="27" t="s">
@@ -19193,7 +19192,7 @@
         <v>1017</v>
       </c>
       <c r="C407" s="18" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="D407" s="27"/>
       <c r="E407" s="27" t="s">
@@ -19320,7 +19319,7 @@
         <v>1017</v>
       </c>
       <c r="C412" s="18" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D412" s="27"/>
       <c r="E412" s="27" t="s">
@@ -19845,7 +19844,7 @@
         <v>1022</v>
       </c>
       <c r="C433" s="18" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="D433" s="27"/>
       <c r="E433" s="27" t="s">
@@ -20172,7 +20171,7 @@
         <v>1025</v>
       </c>
       <c r="C446" s="18" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="D446" s="27"/>
       <c r="E446" s="27" t="s">
@@ -20247,7 +20246,7 @@
         <v>1025</v>
       </c>
       <c r="C449" s="18" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="D449" s="27"/>
       <c r="E449" s="27" t="s">
@@ -20822,7 +20821,7 @@
         <v>1032</v>
       </c>
       <c r="C472" s="18" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="D472" s="27"/>
       <c r="E472" s="27" t="s">
@@ -20897,7 +20896,7 @@
         <v>1033</v>
       </c>
       <c r="C475" s="18" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="D475" s="27"/>
       <c r="E475" s="27" t="s">
@@ -20999,7 +20998,7 @@
         <v>1033</v>
       </c>
       <c r="C479" s="18" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="D479" s="27"/>
       <c r="E479" s="27" t="s">
@@ -21024,7 +21023,7 @@
         <v>1033</v>
       </c>
       <c r="C480" s="18" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="D480" s="27"/>
       <c r="E480" s="27" t="s">
@@ -21499,7 +21498,7 @@
         <v>1039</v>
       </c>
       <c r="C499" s="18" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="D499" s="27"/>
       <c r="E499" s="27" t="s">
@@ -21518,13 +21517,13 @@
     </row>
     <row r="500" spans="1:9" ht="30">
       <c r="A500" s="20" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B500" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C500" s="18" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="D500" s="31"/>
       <c r="E500" s="31" t="s">
@@ -21549,7 +21548,7 @@
         <v>1039</v>
       </c>
       <c r="C501" s="18" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="D501" s="27"/>
       <c r="E501" s="27" t="s">
@@ -21649,13 +21648,13 @@
     </row>
     <row r="505" spans="1:9" ht="90">
       <c r="A505" s="20" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B505" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C505" s="18" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="D505" s="31"/>
       <c r="E505" s="31" t="s">
@@ -21671,21 +21670,21 @@
         <v>17</v>
       </c>
       <c r="I505" s="32" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="506" spans="1:9" ht="45">
       <c r="A506" s="20" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B506" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C506" s="18" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="D506" s="31" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E506" s="31" t="s">
         <v>19</v>
@@ -21703,16 +21702,16 @@
     </row>
     <row r="507" spans="1:9" ht="90">
       <c r="A507" s="20" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B507" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C507" s="18" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="D507" s="31" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E507" s="31" t="s">
         <v>19</v>
@@ -21736,7 +21735,7 @@
         <v>1039</v>
       </c>
       <c r="C508" s="18" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="D508" s="27"/>
       <c r="E508" s="27" t="s">
@@ -21836,13 +21835,13 @@
     </row>
     <row r="512" spans="1:9" ht="60">
       <c r="A512" s="20" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B512" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C512" s="18" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D512" s="31"/>
       <c r="E512" s="27" t="s">
@@ -21858,21 +21857,21 @@
         <v>17</v>
       </c>
       <c r="I512" s="32" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="513" spans="1:9" ht="45">
       <c r="A513" s="31" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B513" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C513" s="18" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="D513" s="31" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E513" s="27" t="s">
         <v>19</v>
@@ -21890,16 +21889,16 @@
     </row>
     <row r="514" spans="1:9" ht="45">
       <c r="A514" s="31" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B514" s="28" t="s">
         <v>1039</v>
       </c>
       <c r="C514" s="18" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D514" s="31" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E514" s="27" t="s">
         <v>19</v>
@@ -21923,7 +21922,7 @@
         <v>1039</v>
       </c>
       <c r="C515" s="18" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="D515" s="27"/>
       <c r="E515" s="27" t="s">
@@ -22348,7 +22347,7 @@
         <v>1041</v>
       </c>
       <c r="C532" s="18" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="D532" s="27"/>
       <c r="E532" s="27" t="s">
@@ -22373,7 +22372,7 @@
         <v>1041</v>
       </c>
       <c r="C533" s="18" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="D533" s="27"/>
       <c r="E533" s="27" t="s">
@@ -22398,7 +22397,7 @@
         <v>1042</v>
       </c>
       <c r="C534" s="18" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="D534" s="27"/>
       <c r="E534" s="27" t="s">
@@ -22448,7 +22447,7 @@
         <v>1043</v>
       </c>
       <c r="C536" s="18" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="D536" s="27"/>
       <c r="E536" s="27" t="s">
@@ -22523,7 +22522,7 @@
         <v>1044</v>
       </c>
       <c r="C539" s="18" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="D539" s="27"/>
       <c r="E539" s="27" t="s">
@@ -22548,7 +22547,7 @@
         <v>1044</v>
       </c>
       <c r="C540" s="18" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
       <c r="D540" s="27"/>
       <c r="E540" s="27" t="s">
@@ -22573,7 +22572,7 @@
         <v>1045</v>
       </c>
       <c r="C541" s="18" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D541" s="27"/>
       <c r="E541" s="27" t="s">
@@ -22598,7 +22597,7 @@
         <v>1045</v>
       </c>
       <c r="C542" s="18" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="D542" s="27"/>
       <c r="E542" s="27" t="s">
@@ -22673,7 +22672,7 @@
         <v>1046</v>
       </c>
       <c r="C545" s="18" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D545" s="27"/>
       <c r="E545" s="27" t="s">
@@ -23252,7 +23251,7 @@
         <v>1053</v>
       </c>
       <c r="C568" s="18" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="D568" s="27"/>
       <c r="E568" s="27" t="s">
@@ -23402,7 +23401,7 @@
         <v>1054</v>
       </c>
       <c r="C574" s="18" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="D574" s="27"/>
       <c r="E574" s="27" t="s">
@@ -23829,7 +23828,7 @@
         <v>1059</v>
       </c>
       <c r="C591" s="18" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D591" s="27"/>
       <c r="E591" s="27" t="s">
@@ -23873,13 +23872,13 @@
     </row>
     <row r="593" spans="1:9" ht="30">
       <c r="A593" s="31" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B593" s="28" t="s">
         <v>1059</v>
       </c>
       <c r="C593" s="32" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D593" s="31"/>
       <c r="E593" s="31" t="s">
@@ -24029,7 +24028,7 @@
         <v>1061</v>
       </c>
       <c r="C599" s="18" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
       <c r="D599" s="27"/>
       <c r="E599" s="27" t="s">
@@ -24131,7 +24130,7 @@
         <v>1061</v>
       </c>
       <c r="C603" s="18" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="D603" s="27"/>
       <c r="E603" s="27" t="s">
@@ -24506,7 +24505,7 @@
         <v>1068</v>
       </c>
       <c r="C618" s="18" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="D618" s="27"/>
       <c r="E618" s="27" t="s">
@@ -24883,7 +24882,7 @@
         <v>1073</v>
       </c>
       <c r="C633" s="18" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="D633" s="27"/>
       <c r="E633" s="27" t="s">
@@ -25110,7 +25109,7 @@
         <v>1075</v>
       </c>
       <c r="C642" s="18" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
       <c r="D642" s="27"/>
       <c r="E642" s="27" t="s">
@@ -25587,7 +25586,7 @@
         <v>1080</v>
       </c>
       <c r="C661" s="18" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="D661" s="27"/>
       <c r="E661" s="27" t="s">
@@ -25712,7 +25711,7 @@
         <v>1081</v>
       </c>
       <c r="C666" s="18" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D666" s="27"/>
       <c r="E666" s="27" t="s">
@@ -25737,7 +25736,7 @@
         <v>1081</v>
       </c>
       <c r="C667" s="18" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="D667" s="27"/>
       <c r="E667" s="27" t="s">
@@ -25789,7 +25788,7 @@
         <v>1082</v>
       </c>
       <c r="C669" s="18" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
       <c r="D669" s="27"/>
       <c r="E669" s="27" t="s">
@@ -25816,7 +25815,7 @@
         <v>1082</v>
       </c>
       <c r="C670" s="18" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="D670" s="27"/>
       <c r="E670" s="27" t="s">
@@ -25841,7 +25840,7 @@
         <v>1082</v>
       </c>
       <c r="C671" s="18" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="D671" s="27"/>
       <c r="E671" s="27" t="s">
@@ -26991,7 +26990,7 @@
         <v>1087</v>
       </c>
       <c r="C717" s="18" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D717" s="27"/>
       <c r="E717" s="27" t="s">
@@ -27010,13 +27009,13 @@
     </row>
     <row r="718" spans="1:9" ht="30">
       <c r="A718" s="20" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B718" s="22" t="s">
         <v>1087</v>
       </c>
       <c r="C718" s="32" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D718" s="31"/>
       <c r="E718" s="27" t="s">
@@ -27035,13 +27034,13 @@
     </row>
     <row r="719" spans="1:9" ht="30">
       <c r="A719" s="20" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B719" s="22" t="s">
         <v>1087</v>
       </c>
       <c r="C719" s="32" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D719" s="31"/>
       <c r="E719" s="27" t="s">
@@ -27060,13 +27059,13 @@
     </row>
     <row r="720" spans="1:9" ht="30">
       <c r="A720" s="20" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B720" s="22" t="s">
         <v>1087</v>
       </c>
       <c r="C720" s="32" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D720" s="31"/>
       <c r="E720" s="27" t="s">
@@ -27085,13 +27084,13 @@
     </row>
     <row r="721" spans="1:9" ht="30">
       <c r="A721" s="20" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B721" s="22" t="s">
         <v>1087</v>
       </c>
       <c r="C721" s="18" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="D721" s="31"/>
       <c r="E721" s="27" t="s">
@@ -27116,7 +27115,7 @@
         <v>1088</v>
       </c>
       <c r="C722" s="18" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D722" s="27"/>
       <c r="E722" s="27" t="s">
@@ -27466,7 +27465,7 @@
         <v>1088</v>
       </c>
       <c r="C736" s="18" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D736" s="27"/>
       <c r="E736" s="27" t="s">
@@ -27491,7 +27490,7 @@
         <v>1088</v>
       </c>
       <c r="C737" s="18" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D737" s="27"/>
       <c r="E737" s="27" t="s">
@@ -27510,13 +27509,13 @@
     </row>
     <row r="738" spans="1:9" ht="30">
       <c r="A738" s="20" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B738" s="28" t="s">
         <v>1088</v>
       </c>
       <c r="C738" s="32" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D738" s="31"/>
       <c r="E738" s="31" t="s">
@@ -27793,7 +27792,7 @@
         <v>1089</v>
       </c>
       <c r="C749" s="18" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="D749" s="27"/>
       <c r="E749" s="27" t="s">
@@ -28445,7 +28444,7 @@
         <v>1094</v>
       </c>
       <c r="C775" s="18" t="s">
-        <v>2019</v>
+        <v>2158</v>
       </c>
       <c r="D775" s="27"/>
       <c r="E775" s="27" t="s">
@@ -28489,13 +28488,13 @@
     </row>
     <row r="777" spans="1:9" ht="30">
       <c r="A777" s="20" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B777" s="28" t="s">
         <v>1094</v>
       </c>
       <c r="C777" s="32" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D777" s="31"/>
       <c r="E777" s="31" t="s">
@@ -29520,7 +29519,7 @@
         <v>1096</v>
       </c>
       <c r="C818" s="18" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="D818" s="27"/>
       <c r="E818" s="27" t="s">
@@ -29997,7 +29996,7 @@
         <v>1101</v>
       </c>
       <c r="C837" s="18" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D837" s="27"/>
       <c r="E837" s="27" t="s">
@@ -30041,13 +30040,13 @@
     </row>
     <row r="839" spans="1:9" ht="30">
       <c r="A839" s="20" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="B839" s="28" t="s">
         <v>1101</v>
       </c>
       <c r="C839" s="32" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D839" s="31"/>
       <c r="E839" s="27" t="s">
@@ -30322,7 +30321,7 @@
         <v>1102</v>
       </c>
       <c r="C850" s="18" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D850" s="27"/>
       <c r="E850" s="27" t="s">
@@ -30397,7 +30396,7 @@
         <v>1103</v>
       </c>
       <c r="C853" s="18" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="D853" s="27"/>
       <c r="E853" s="27" t="s">
@@ -30472,7 +30471,7 @@
         <v>1103</v>
       </c>
       <c r="C856" s="18" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="D856" s="27"/>
       <c r="E856" s="27" t="s">
@@ -30497,7 +30496,7 @@
         <v>1103</v>
       </c>
       <c r="C857" s="18" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
       <c r="D857" s="27"/>
       <c r="E857" s="27" t="s">
@@ -30547,7 +30546,7 @@
         <v>1104</v>
       </c>
       <c r="C859" s="18" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="D859" s="27"/>
       <c r="E859" s="27" t="s">
@@ -30572,7 +30571,7 @@
         <v>1104</v>
       </c>
       <c r="C860" s="18" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="D860" s="27"/>
       <c r="E860" s="27" t="s">
@@ -30597,7 +30596,7 @@
         <v>1105</v>
       </c>
       <c r="C861" s="18" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="D861" s="27"/>
       <c r="E861" s="27" t="s">
@@ -30672,7 +30671,7 @@
         <v>1106</v>
       </c>
       <c r="C864" s="18" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="D864" s="27"/>
       <c r="E864" s="27" t="s">
@@ -30822,7 +30821,7 @@
         <v>1108</v>
       </c>
       <c r="C870" s="18" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D870" s="27"/>
       <c r="E870" s="27" t="s">
@@ -30847,7 +30846,7 @@
         <v>1108</v>
       </c>
       <c r="C871" s="18" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="D871" s="27"/>
       <c r="E871" s="27" t="s">
@@ -30897,7 +30896,7 @@
         <v>1109</v>
       </c>
       <c r="C873" s="18" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="D873" s="27"/>
       <c r="E873" s="27" t="s">
@@ -30922,7 +30921,7 @@
         <v>1109</v>
       </c>
       <c r="C874" s="18" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="D874" s="27"/>
       <c r="E874" s="27" t="s">
@@ -31109,7 +31108,7 @@
         <v>7</v>
       </c>
       <c r="C881" s="18" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="D881" s="20" t="s">
         <v>1840</v>
@@ -31132,16 +31131,16 @@
     </row>
     <row r="882" spans="1:9" ht="45">
       <c r="A882" s="20" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="B882" s="22" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="C882" s="18" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="D882" s="20" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="E882" s="27" t="s">
         <v>22</v>
@@ -31159,16 +31158,16 @@
     </row>
     <row r="883" spans="1:9" ht="45">
       <c r="A883" s="20" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="B883" s="22" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="C883" s="18" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="D883" s="20" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="E883" s="27" t="s">
         <v>22</v>
@@ -31188,16 +31187,16 @@
     </row>
     <row r="884" spans="1:9" ht="60">
       <c r="A884" s="20" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="B884" s="22" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="C884" s="18" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="D884" s="20" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="E884" s="27" t="s">
         <v>22</v>
@@ -31215,16 +31214,16 @@
     </row>
     <row r="885" spans="1:9" ht="45">
       <c r="A885" s="20" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="B885" s="22" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="C885" s="18" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="D885" s="20" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="E885" s="27" t="s">
         <v>22</v>
@@ -31250,7 +31249,7 @@
         <v>7</v>
       </c>
       <c r="C886" s="18" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="D886" s="20" t="s">
         <v>1841</v>
@@ -31277,7 +31276,7 @@
         <v>7</v>
       </c>
       <c r="C887" s="18" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="D887" s="20" t="s">
         <v>1841</v>
@@ -31306,7 +31305,7 @@
         <v>7</v>
       </c>
       <c r="C888" s="18" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="D888" s="20" t="s">
         <v>1842</v>
@@ -31333,7 +31332,7 @@
         <v>7</v>
       </c>
       <c r="C889" s="18" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="D889" s="20" t="s">
         <v>1842</v>
@@ -31362,7 +31361,7 @@
         <v>7</v>
       </c>
       <c r="C890" s="18" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="D890" s="20" t="s">
         <v>1843</v>
@@ -31389,7 +31388,7 @@
         <v>7</v>
       </c>
       <c r="C891" s="18" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="D891" s="20" t="s">
         <v>1843</v>
@@ -31418,7 +31417,7 @@
         <v>7</v>
       </c>
       <c r="C892" s="18" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="D892" s="20" t="s">
         <v>1844</v>
@@ -31445,7 +31444,7 @@
         <v>7</v>
       </c>
       <c r="C893" s="18" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
       <c r="D893" s="20" t="s">
         <v>1844</v>
@@ -31474,7 +31473,7 @@
         <v>7</v>
       </c>
       <c r="C894" s="18" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="D894" s="20" t="s">
         <v>1837</v>
@@ -31501,7 +31500,7 @@
         <v>7</v>
       </c>
       <c r="C895" s="18" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="D895" s="20" t="s">
         <v>1837</v>
@@ -31530,7 +31529,7 @@
         <v>7</v>
       </c>
       <c r="C896" s="18" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="D896" s="20" t="s">
         <v>1838</v>
@@ -31557,7 +31556,7 @@
         <v>7</v>
       </c>
       <c r="C897" s="18" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="D897" s="27"/>
       <c r="E897" s="27" t="s">
@@ -31582,7 +31581,7 @@
         <v>7</v>
       </c>
       <c r="C898" s="18" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="D898" s="27"/>
       <c r="E898" s="27" t="s">
@@ -31632,7 +31631,7 @@
         <v>7</v>
       </c>
       <c r="C900" s="18" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="D900" s="27"/>
       <c r="E900" s="27" t="s">
@@ -31782,7 +31781,7 @@
         <v>7</v>
       </c>
       <c r="C906" s="18" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="D906" s="27"/>
       <c r="E906" s="27" t="s">
@@ -31807,7 +31806,7 @@
         <v>7</v>
       </c>
       <c r="C907" s="18" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="D907" s="27"/>
       <c r="E907" s="27" t="s">
@@ -31876,13 +31875,13 @@
     </row>
     <row r="910" spans="1:9" ht="75">
       <c r="A910" s="20" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="B910" s="35" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="C910" s="32" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="D910" s="31"/>
       <c r="E910" s="27" t="s">
@@ -31901,13 +31900,13 @@
     </row>
     <row r="911" spans="1:9" ht="75">
       <c r="A911" s="20" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="B911" s="35" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="C911" s="32" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="D911" s="31"/>
       <c r="E911" s="27" t="s">
@@ -31932,7 +31931,7 @@
         <v>7</v>
       </c>
       <c r="C912" s="18" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="D912" s="20" t="s">
         <v>1845</v>
@@ -31959,7 +31958,7 @@
         <v>7</v>
       </c>
       <c r="C913" s="18" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
       <c r="D913" s="20" t="s">
         <v>1845</v>
@@ -31988,7 +31987,7 @@
         <v>7</v>
       </c>
       <c r="C914" s="18" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D914" s="20" t="s">
         <v>1846</v>
@@ -32015,7 +32014,7 @@
         <v>7</v>
       </c>
       <c r="C915" s="18" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
       <c r="D915" s="20" t="s">
         <v>1847</v>
@@ -32042,7 +32041,7 @@
         <v>7</v>
       </c>
       <c r="C916" s="18" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="D916" s="27" t="s">
         <v>1847</v>
@@ -32071,7 +32070,7 @@
         <v>7</v>
       </c>
       <c r="C917" s="18" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
       <c r="D917" s="27" t="s">
         <v>1846</v>
@@ -32100,7 +32099,7 @@
         <v>7</v>
       </c>
       <c r="C918" s="18" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="D918" s="27" t="s">
         <v>1848</v>
@@ -32127,7 +32126,7 @@
         <v>7</v>
       </c>
       <c r="C919" s="18" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
       <c r="D919" s="27" t="s">
         <v>1848</v>
@@ -32156,7 +32155,7 @@
         <v>7</v>
       </c>
       <c r="C920" s="18" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
       <c r="D920" s="27" t="s">
         <v>1838</v>
@@ -32183,7 +32182,7 @@
         <v>7</v>
       </c>
       <c r="C921" s="18" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
       <c r="D921" s="27" t="s">
         <v>1849</v>
@@ -32210,7 +32209,7 @@
         <v>7</v>
       </c>
       <c r="C922" s="18" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
       <c r="D922" s="27" t="s">
         <v>1849</v>
@@ -32239,7 +32238,7 @@
         <v>7</v>
       </c>
       <c r="C923" s="18" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="D923" s="27" t="s">
         <v>1850</v>
@@ -32266,7 +32265,7 @@
         <v>7</v>
       </c>
       <c r="C924" s="18" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="D924" s="27" t="s">
         <v>1850</v>
@@ -32293,7 +32292,7 @@
         <v>7</v>
       </c>
       <c r="C925" s="18" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="D925" s="27" t="s">
         <v>1851</v>
@@ -32320,7 +32319,7 @@
         <v>7</v>
       </c>
       <c r="C926" s="18" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
       <c r="D926" s="27" t="s">
         <v>1851</v>
@@ -32347,7 +32346,7 @@
         <v>7</v>
       </c>
       <c r="C927" s="18" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="D927" s="27" t="s">
         <v>1852</v>
@@ -32374,7 +32373,7 @@
         <v>7</v>
       </c>
       <c r="C928" s="18" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="D928" s="27" t="s">
         <v>1852</v>
@@ -32403,7 +32402,7 @@
         <v>7</v>
       </c>
       <c r="C929" s="18" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D929" s="27" t="s">
         <v>1853</v>
@@ -32430,7 +32429,7 @@
         <v>7</v>
       </c>
       <c r="C930" s="18" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="D930" s="27" t="s">
         <v>1853</v>
@@ -32459,7 +32458,7 @@
         <v>7</v>
       </c>
       <c r="C931" s="18" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="D931" s="27" t="s">
         <v>1854</v>
@@ -32486,7 +32485,7 @@
         <v>7</v>
       </c>
       <c r="C932" s="18" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="D932" s="27" t="s">
         <v>1854</v>
@@ -32515,7 +32514,7 @@
         <v>7</v>
       </c>
       <c r="C933" s="18" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="D933" s="27" t="s">
         <v>1855</v>
@@ -32542,7 +32541,7 @@
         <v>7</v>
       </c>
       <c r="C934" s="18" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="D934" s="27" t="s">
         <v>1855</v>
@@ -32571,7 +32570,7 @@
         <v>7</v>
       </c>
       <c r="C935" s="18" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
       <c r="D935" s="27" t="s">
         <v>1856</v>
@@ -32598,7 +32597,7 @@
         <v>7</v>
       </c>
       <c r="C936" s="18" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="D936" s="27" t="s">
         <v>1856</v>
@@ -32627,7 +32626,7 @@
         <v>7</v>
       </c>
       <c r="C937" s="18" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="D937" s="27" t="s">
         <v>1857</v>
@@ -32654,7 +32653,7 @@
         <v>7</v>
       </c>
       <c r="C938" s="18" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
       <c r="D938" s="27" t="s">
         <v>1857</v>
@@ -32683,7 +32682,7 @@
         <v>7</v>
       </c>
       <c r="C939" s="18" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
       <c r="D939" s="27" t="s">
         <v>1858</v>
@@ -32710,7 +32709,7 @@
         <v>7</v>
       </c>
       <c r="C940" s="18" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="D940" s="27" t="s">
         <v>1858</v>
@@ -33278,6 +33277,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -33285,11 +33289,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A689:B689 E942:E945 D689:I689 A877:H877 A946:I959 I669:I877 A690:I876 A20:I688 A878:I941">
@@ -33398,7 +33397,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B18:B27 B10:B16 B886:B959 C3 B28:B55 B59:B881" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B18:B27 B10:B16 B886:B959 B28:B55 B59:B881" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -33414,15 +33413,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -33471,6 +33461,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -33486,14 +33485,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33506,4 +33497,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>